<commit_message>
Implement Autoplay Preview feature with double-click to queue functionality
</commit_message>
<xml_diff>
--- a/doc/Layout.xlsx
+++ b/doc/Layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Arma3\Modding\ZeusJukebox\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Arma 3 Modding\21_ZeusJukebox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9053718C-D0D6-4B01-98F6-3EAB8D48534D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA780D5D-3559-45B7-B783-229FA0D7AEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{682E6184-E15B-4402-836A-91257A3551C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{682E6184-E15B-4402-836A-91257A3551C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>*</t>
   </si>
@@ -137,9 +137,6 @@
     <t>AutoplayBtn</t>
   </si>
   <si>
-    <t>Autoplay:</t>
-  </si>
-  <si>
     <t>Play</t>
   </si>
   <si>
@@ -153,6 +150,12 @@
   </si>
   <si>
     <t>Zeus Jukebox Logs</t>
+  </si>
+  <si>
+    <t>Autoplay Preview:</t>
+  </si>
+  <si>
+    <t>Autoplay Global Music:</t>
   </si>
 </sst>
 </file>
@@ -471,22 +474,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -834,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5B835F-835A-4242-BD99-7FE00DEEB233}">
   <dimension ref="A1:DH112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT94" sqref="AT94"/>
+    <sheetView tabSelected="1" topLeftCell="O34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="CV49" sqref="CV49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.140625" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2577,21 +2580,22 @@
       <c r="BE18" s="20"/>
       <c r="BF18" s="20"/>
       <c r="BG18" s="20"/>
-      <c r="BH18" s="20"/>
-      <c r="BI18" s="20"/>
-      <c r="BJ18" s="20"/>
       <c r="BK18" s="20"/>
-      <c r="BL18" s="20"/>
-      <c r="BM18" s="20"/>
-      <c r="BN18" s="20"/>
-      <c r="BO18" s="20"/>
-      <c r="BP18" s="20"/>
-      <c r="BQ18" s="20"/>
-      <c r="BR18" s="20"/>
-      <c r="BS18" s="20"/>
-      <c r="BT18" s="20"/>
-      <c r="BU18" s="20"/>
-      <c r="BV18" s="20"/>
+      <c r="BL18" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="BM18" s="31"/>
+      <c r="BN18" s="31"/>
+      <c r="BO18" s="31"/>
+      <c r="BP18" s="31"/>
+      <c r="BQ18" s="32"/>
+      <c r="BR18" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="BS18" s="31"/>
+      <c r="BT18" s="31"/>
+      <c r="BU18" s="31"/>
+      <c r="BV18" s="32"/>
       <c r="BX18" s="24" t="s">
         <v>4</v>
       </c>
@@ -2677,21 +2681,18 @@
       <c r="BE19" s="20"/>
       <c r="BF19" s="20"/>
       <c r="BG19" s="20"/>
-      <c r="BH19" s="20"/>
-      <c r="BI19" s="20"/>
-      <c r="BJ19" s="20"/>
       <c r="BK19" s="20"/>
-      <c r="BL19" s="20"/>
-      <c r="BM19" s="20"/>
-      <c r="BN19" s="20"/>
-      <c r="BO19" s="20"/>
-      <c r="BP19" s="20"/>
-      <c r="BQ19" s="20"/>
-      <c r="BR19" s="20"/>
-      <c r="BS19" s="20"/>
-      <c r="BT19" s="20"/>
-      <c r="BU19" s="20"/>
-      <c r="BV19" s="20"/>
+      <c r="BL19" s="33"/>
+      <c r="BM19" s="34"/>
+      <c r="BN19" s="34"/>
+      <c r="BO19" s="34"/>
+      <c r="BP19" s="34"/>
+      <c r="BQ19" s="35"/>
+      <c r="BR19" s="33"/>
+      <c r="BS19" s="34"/>
+      <c r="BT19" s="34"/>
+      <c r="BU19" s="34"/>
+      <c r="BV19" s="35"/>
       <c r="BX19" s="27"/>
       <c r="BY19" s="28"/>
       <c r="BZ19" s="28"/>
@@ -2920,14 +2921,14 @@
       <c r="BZ22" s="25"/>
       <c r="CA22" s="25"/>
       <c r="CB22" s="26"/>
-      <c r="CF22" s="34" t="s">
+      <c r="CF22" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="CG22" s="31"/>
-      <c r="CJ22" s="34" t="s">
+      <c r="CG22" s="32"/>
+      <c r="CJ22" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="CK22" s="31"/>
+      <c r="CK22" s="32"/>
       <c r="CL22" s="13"/>
       <c r="CM22" s="13"/>
       <c r="CN22" s="2">
@@ -3004,10 +3005,10 @@
       <c r="BZ23" s="28"/>
       <c r="CA23" s="28"/>
       <c r="CB23" s="29"/>
-      <c r="CF23" s="35"/>
-      <c r="CG23" s="33"/>
-      <c r="CJ23" s="35"/>
-      <c r="CK23" s="33"/>
+      <c r="CF23" s="33"/>
+      <c r="CG23" s="35"/>
+      <c r="CJ23" s="33"/>
+      <c r="CK23" s="35"/>
       <c r="CL23" s="13"/>
       <c r="CM23" s="13"/>
       <c r="CN23" s="2">
@@ -3101,40 +3102,40 @@
       <c r="AL25" s="26"/>
       <c r="AM25" s="13"/>
       <c r="AO25" s="12"/>
-      <c r="AP25" s="34" t="s">
+      <c r="AP25" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="AQ25" s="30"/>
-      <c r="AR25" s="30"/>
-      <c r="AS25" s="30"/>
-      <c r="AT25" s="30"/>
-      <c r="AU25" s="30"/>
-      <c r="AV25" s="30"/>
-      <c r="AW25" s="30"/>
-      <c r="AX25" s="30"/>
-      <c r="AY25" s="30"/>
-      <c r="AZ25" s="30"/>
-      <c r="BA25" s="30"/>
-      <c r="BB25" s="30"/>
-      <c r="BC25" s="30"/>
-      <c r="BD25" s="30"/>
-      <c r="BE25" s="30"/>
-      <c r="BF25" s="30"/>
-      <c r="BG25" s="30"/>
-      <c r="BH25" s="30"/>
-      <c r="BI25" s="30"/>
-      <c r="BJ25" s="30"/>
-      <c r="BK25" s="30"/>
-      <c r="BL25" s="30"/>
-      <c r="BM25" s="30"/>
-      <c r="BN25" s="30"/>
-      <c r="BO25" s="30"/>
-      <c r="BP25" s="30"/>
-      <c r="BQ25" s="30"/>
-      <c r="BR25" s="30"/>
-      <c r="BS25" s="30"/>
-      <c r="BT25" s="30"/>
-      <c r="BU25" s="31"/>
+      <c r="AQ25" s="31"/>
+      <c r="AR25" s="31"/>
+      <c r="AS25" s="31"/>
+      <c r="AT25" s="31"/>
+      <c r="AU25" s="31"/>
+      <c r="AV25" s="31"/>
+      <c r="AW25" s="31"/>
+      <c r="AX25" s="31"/>
+      <c r="AY25" s="31"/>
+      <c r="AZ25" s="31"/>
+      <c r="BA25" s="31"/>
+      <c r="BB25" s="31"/>
+      <c r="BC25" s="31"/>
+      <c r="BD25" s="31"/>
+      <c r="BE25" s="31"/>
+      <c r="BF25" s="31"/>
+      <c r="BG25" s="31"/>
+      <c r="BH25" s="31"/>
+      <c r="BI25" s="31"/>
+      <c r="BJ25" s="31"/>
+      <c r="BK25" s="31"/>
+      <c r="BL25" s="31"/>
+      <c r="BM25" s="31"/>
+      <c r="BN25" s="31"/>
+      <c r="BO25" s="31"/>
+      <c r="BP25" s="31"/>
+      <c r="BQ25" s="31"/>
+      <c r="BR25" s="31"/>
+      <c r="BS25" s="31"/>
+      <c r="BT25" s="31"/>
+      <c r="BU25" s="32"/>
       <c r="BV25" s="13"/>
       <c r="BX25" s="12"/>
       <c r="CL25" s="13"/>
@@ -3188,38 +3189,38 @@
       <c r="AL26" s="29"/>
       <c r="AM26" s="13"/>
       <c r="AO26" s="12"/>
-      <c r="AP26" s="35"/>
-      <c r="AQ26" s="32"/>
-      <c r="AR26" s="32"/>
-      <c r="AS26" s="32"/>
-      <c r="AT26" s="32"/>
-      <c r="AU26" s="32"/>
-      <c r="AV26" s="32"/>
-      <c r="AW26" s="32"/>
-      <c r="AX26" s="32"/>
-      <c r="AY26" s="32"/>
-      <c r="AZ26" s="32"/>
-      <c r="BA26" s="32"/>
-      <c r="BB26" s="32"/>
-      <c r="BC26" s="32"/>
-      <c r="BD26" s="32"/>
-      <c r="BE26" s="32"/>
-      <c r="BF26" s="32"/>
-      <c r="BG26" s="32"/>
-      <c r="BH26" s="32"/>
-      <c r="BI26" s="32"/>
-      <c r="BJ26" s="32"/>
-      <c r="BK26" s="32"/>
-      <c r="BL26" s="32"/>
-      <c r="BM26" s="32"/>
-      <c r="BN26" s="32"/>
-      <c r="BO26" s="32"/>
-      <c r="BP26" s="32"/>
-      <c r="BQ26" s="32"/>
-      <c r="BR26" s="32"/>
-      <c r="BS26" s="32"/>
-      <c r="BT26" s="32"/>
-      <c r="BU26" s="33"/>
+      <c r="AP26" s="33"/>
+      <c r="AQ26" s="34"/>
+      <c r="AR26" s="34"/>
+      <c r="AS26" s="34"/>
+      <c r="AT26" s="34"/>
+      <c r="AU26" s="34"/>
+      <c r="AV26" s="34"/>
+      <c r="AW26" s="34"/>
+      <c r="AX26" s="34"/>
+      <c r="AY26" s="34"/>
+      <c r="AZ26" s="34"/>
+      <c r="BA26" s="34"/>
+      <c r="BB26" s="34"/>
+      <c r="BC26" s="34"/>
+      <c r="BD26" s="34"/>
+      <c r="BE26" s="34"/>
+      <c r="BF26" s="34"/>
+      <c r="BG26" s="34"/>
+      <c r="BH26" s="34"/>
+      <c r="BI26" s="34"/>
+      <c r="BJ26" s="34"/>
+      <c r="BK26" s="34"/>
+      <c r="BL26" s="34"/>
+      <c r="BM26" s="34"/>
+      <c r="BN26" s="34"/>
+      <c r="BO26" s="34"/>
+      <c r="BP26" s="34"/>
+      <c r="BQ26" s="34"/>
+      <c r="BR26" s="34"/>
+      <c r="BS26" s="34"/>
+      <c r="BT26" s="34"/>
+      <c r="BU26" s="35"/>
       <c r="BV26" s="13"/>
       <c r="BX26" s="12"/>
       <c r="CL26" s="13"/>
@@ -3342,22 +3343,22 @@
       <c r="BN28" s="20"/>
       <c r="BV28" s="13"/>
       <c r="BX28" s="12"/>
-      <c r="BY28" s="34" t="s">
+      <c r="BY28" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="BZ28" s="30"/>
-      <c r="CA28" s="30"/>
-      <c r="CB28" s="30"/>
-      <c r="CC28" s="30"/>
-      <c r="CD28" s="31"/>
-      <c r="CF28" s="34" t="s">
+      <c r="BZ28" s="31"/>
+      <c r="CA28" s="31"/>
+      <c r="CB28" s="31"/>
+      <c r="CC28" s="31"/>
+      <c r="CD28" s="32"/>
+      <c r="CF28" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="CG28" s="30"/>
-      <c r="CH28" s="30"/>
-      <c r="CI28" s="30"/>
-      <c r="CJ28" s="30"/>
-      <c r="CK28" s="31"/>
+      <c r="CG28" s="31"/>
+      <c r="CH28" s="31"/>
+      <c r="CI28" s="31"/>
+      <c r="CJ28" s="31"/>
+      <c r="CK28" s="32"/>
       <c r="CL28" s="13"/>
       <c r="CM28" s="13"/>
       <c r="CN28" s="2">
@@ -3434,18 +3435,18 @@
       <c r="BN29" s="20"/>
       <c r="BV29" s="13"/>
       <c r="BX29" s="12"/>
-      <c r="BY29" s="35"/>
-      <c r="BZ29" s="32"/>
-      <c r="CA29" s="32"/>
-      <c r="CB29" s="32"/>
-      <c r="CC29" s="32"/>
-      <c r="CD29" s="33"/>
-      <c r="CF29" s="35"/>
-      <c r="CG29" s="32"/>
-      <c r="CH29" s="32"/>
-      <c r="CI29" s="32"/>
-      <c r="CJ29" s="32"/>
-      <c r="CK29" s="33"/>
+      <c r="BY29" s="33"/>
+      <c r="BZ29" s="34"/>
+      <c r="CA29" s="34"/>
+      <c r="CB29" s="34"/>
+      <c r="CC29" s="34"/>
+      <c r="CD29" s="35"/>
+      <c r="CF29" s="33"/>
+      <c r="CG29" s="34"/>
+      <c r="CH29" s="34"/>
+      <c r="CI29" s="34"/>
+      <c r="CJ29" s="34"/>
+      <c r="CK29" s="35"/>
       <c r="CL29" s="13"/>
       <c r="CM29" s="13"/>
       <c r="CN29" s="2">
@@ -3560,52 +3561,52 @@
       <c r="AS31" s="20"/>
       <c r="AT31" s="20"/>
       <c r="AU31" s="20"/>
-      <c r="AV31" s="34" t="s">
+      <c r="AV31" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="AW31" s="30"/>
-      <c r="AX31" s="30"/>
-      <c r="AY31" s="30"/>
-      <c r="AZ31" s="30"/>
-      <c r="BA31" s="31"/>
+      <c r="AW31" s="31"/>
+      <c r="AX31" s="31"/>
+      <c r="AY31" s="31"/>
+      <c r="AZ31" s="31"/>
+      <c r="BA31" s="32"/>
       <c r="BB31" s="20"/>
-      <c r="BC31" s="34" t="s">
+      <c r="BC31" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="BD31" s="30"/>
-      <c r="BE31" s="30"/>
-      <c r="BF31" s="30"/>
-      <c r="BG31" s="30"/>
-      <c r="BH31" s="31"/>
+      <c r="BD31" s="31"/>
+      <c r="BE31" s="31"/>
+      <c r="BF31" s="31"/>
+      <c r="BG31" s="31"/>
+      <c r="BH31" s="32"/>
       <c r="BI31" s="20"/>
-      <c r="BJ31" s="34" t="s">
+      <c r="BJ31" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="BK31" s="30"/>
-      <c r="BL31" s="30"/>
-      <c r="BM31" s="30"/>
-      <c r="BN31" s="30"/>
-      <c r="BO31" s="31"/>
+      <c r="BK31" s="31"/>
+      <c r="BL31" s="31"/>
+      <c r="BM31" s="31"/>
+      <c r="BN31" s="31"/>
+      <c r="BO31" s="32"/>
       <c r="BP31" s="20"/>
       <c r="BQ31" s="20"/>
       <c r="BR31" s="20"/>
       <c r="BV31" s="13"/>
       <c r="BX31" s="12"/>
-      <c r="BY31" s="34" t="s">
+      <c r="BY31" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="BZ31" s="30"/>
-      <c r="CA31" s="30"/>
-      <c r="CB31" s="30"/>
-      <c r="CC31" s="30"/>
-      <c r="CD31" s="30"/>
-      <c r="CE31" s="30"/>
-      <c r="CF31" s="30"/>
-      <c r="CG31" s="30"/>
-      <c r="CH31" s="30"/>
-      <c r="CI31" s="30"/>
-      <c r="CJ31" s="30"/>
-      <c r="CK31" s="31"/>
+      <c r="BZ31" s="31"/>
+      <c r="CA31" s="31"/>
+      <c r="CB31" s="31"/>
+      <c r="CC31" s="31"/>
+      <c r="CD31" s="31"/>
+      <c r="CE31" s="31"/>
+      <c r="CF31" s="31"/>
+      <c r="CG31" s="31"/>
+      <c r="CH31" s="31"/>
+      <c r="CI31" s="31"/>
+      <c r="CJ31" s="31"/>
+      <c r="CK31" s="32"/>
       <c r="CL31" s="13"/>
       <c r="CM31" s="13"/>
       <c r="CN31" s="2">
@@ -3660,26 +3661,26 @@
       <c r="AS32" s="20"/>
       <c r="AT32" s="20"/>
       <c r="AU32" s="20"/>
-      <c r="AV32" s="35"/>
-      <c r="AW32" s="32"/>
-      <c r="AX32" s="32"/>
-      <c r="AY32" s="32"/>
-      <c r="AZ32" s="32"/>
-      <c r="BA32" s="33"/>
+      <c r="AV32" s="33"/>
+      <c r="AW32" s="34"/>
+      <c r="AX32" s="34"/>
+      <c r="AY32" s="34"/>
+      <c r="AZ32" s="34"/>
+      <c r="BA32" s="35"/>
       <c r="BB32" s="20"/>
-      <c r="BC32" s="35"/>
-      <c r="BD32" s="32"/>
-      <c r="BE32" s="32"/>
-      <c r="BF32" s="32"/>
-      <c r="BG32" s="32"/>
-      <c r="BH32" s="33"/>
+      <c r="BC32" s="33"/>
+      <c r="BD32" s="34"/>
+      <c r="BE32" s="34"/>
+      <c r="BF32" s="34"/>
+      <c r="BG32" s="34"/>
+      <c r="BH32" s="35"/>
       <c r="BI32" s="20"/>
-      <c r="BJ32" s="35"/>
-      <c r="BK32" s="32"/>
-      <c r="BL32" s="32"/>
-      <c r="BM32" s="32"/>
-      <c r="BN32" s="32"/>
-      <c r="BO32" s="33"/>
+      <c r="BJ32" s="33"/>
+      <c r="BK32" s="34"/>
+      <c r="BL32" s="34"/>
+      <c r="BM32" s="34"/>
+      <c r="BN32" s="34"/>
+      <c r="BO32" s="35"/>
       <c r="BP32" s="20"/>
       <c r="BQ32" s="20"/>
       <c r="BR32" s="20"/>
@@ -3736,19 +3737,19 @@
       <c r="AO33" s="12"/>
       <c r="BV33" s="13"/>
       <c r="BX33" s="12"/>
-      <c r="BY33" s="35"/>
-      <c r="BZ33" s="32"/>
-      <c r="CA33" s="32"/>
-      <c r="CB33" s="32"/>
-      <c r="CC33" s="32"/>
-      <c r="CD33" s="32"/>
-      <c r="CE33" s="32"/>
-      <c r="CF33" s="32"/>
-      <c r="CG33" s="32"/>
-      <c r="CH33" s="32"/>
-      <c r="CI33" s="32"/>
-      <c r="CJ33" s="32"/>
-      <c r="CK33" s="33"/>
+      <c r="BY33" s="33"/>
+      <c r="BZ33" s="34"/>
+      <c r="CA33" s="34"/>
+      <c r="CB33" s="34"/>
+      <c r="CC33" s="34"/>
+      <c r="CD33" s="34"/>
+      <c r="CE33" s="34"/>
+      <c r="CF33" s="34"/>
+      <c r="CG33" s="34"/>
+      <c r="CH33" s="34"/>
+      <c r="CI33" s="34"/>
+      <c r="CJ33" s="34"/>
+      <c r="CK33" s="35"/>
       <c r="CL33" s="13"/>
       <c r="CM33" s="13"/>
       <c r="CN33" s="2">
@@ -3930,33 +3931,33 @@
       </c>
       <c r="AI36" s="25"/>
       <c r="AJ36" s="26"/>
-      <c r="AK36" s="34" t="s">
+      <c r="AK36" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AL36" s="30"/>
-      <c r="AM36" s="30"/>
-      <c r="AN36" s="31"/>
+      <c r="AL36" s="31"/>
+      <c r="AM36" s="31"/>
+      <c r="AN36" s="32"/>
       <c r="AO36" s="20"/>
-      <c r="AP36" s="34" t="s">
+      <c r="AP36" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="AQ36" s="31"/>
+      <c r="AQ36" s="32"/>
       <c r="AS36" s="20"/>
       <c r="AT36" s="24" t="s">
         <v>10</v>
       </c>
       <c r="AU36" s="25"/>
       <c r="AV36" s="26"/>
-      <c r="AW36" s="30" t="s">
+      <c r="AW36" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="AX36" s="30"/>
-      <c r="AY36" s="30"/>
-      <c r="AZ36" s="30"/>
-      <c r="BA36" s="30"/>
-      <c r="BB36" s="30"/>
-      <c r="BC36" s="30"/>
-      <c r="BD36" s="31"/>
+      <c r="AX36" s="31"/>
+      <c r="AY36" s="31"/>
+      <c r="AZ36" s="31"/>
+      <c r="BA36" s="31"/>
+      <c r="BB36" s="31"/>
+      <c r="BC36" s="31"/>
+      <c r="BD36" s="32"/>
       <c r="BF36" s="24" t="s">
         <v>5</v>
       </c>
@@ -4038,25 +4039,25 @@
       <c r="AH37" s="27"/>
       <c r="AI37" s="28"/>
       <c r="AJ37" s="29"/>
-      <c r="AK37" s="35"/>
-      <c r="AL37" s="32"/>
-      <c r="AM37" s="32"/>
-      <c r="AN37" s="33"/>
+      <c r="AK37" s="33"/>
+      <c r="AL37" s="34"/>
+      <c r="AM37" s="34"/>
+      <c r="AN37" s="35"/>
       <c r="AO37" s="20"/>
-      <c r="AP37" s="35"/>
-      <c r="AQ37" s="33"/>
+      <c r="AP37" s="33"/>
+      <c r="AQ37" s="35"/>
       <c r="AS37" s="20"/>
       <c r="AT37" s="27"/>
       <c r="AU37" s="28"/>
       <c r="AV37" s="29"/>
-      <c r="AW37" s="32"/>
-      <c r="AX37" s="32"/>
-      <c r="AY37" s="32"/>
-      <c r="AZ37" s="32"/>
-      <c r="BA37" s="32"/>
-      <c r="BB37" s="32"/>
-      <c r="BC37" s="32"/>
-      <c r="BD37" s="33"/>
+      <c r="AW37" s="34"/>
+      <c r="AX37" s="34"/>
+      <c r="AY37" s="34"/>
+      <c r="AZ37" s="34"/>
+      <c r="BA37" s="34"/>
+      <c r="BB37" s="34"/>
+      <c r="BC37" s="34"/>
+      <c r="BD37" s="35"/>
       <c r="BF37" s="27"/>
       <c r="BG37" s="28"/>
       <c r="BH37" s="28"/>
@@ -4278,20 +4279,20 @@
       <c r="BX40" s="25"/>
       <c r="BY40" s="26"/>
       <c r="BZ40" s="20"/>
-      <c r="CA40" s="34" t="s">
+      <c r="CA40" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="CB40" s="30"/>
-      <c r="CC40" s="30"/>
-      <c r="CD40" s="30"/>
-      <c r="CE40" s="31"/>
-      <c r="CG40" s="34" t="s">
+      <c r="CB40" s="31"/>
+      <c r="CC40" s="31"/>
+      <c r="CD40" s="31"/>
+      <c r="CE40" s="32"/>
+      <c r="CG40" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="CH40" s="30"/>
-      <c r="CI40" s="30"/>
-      <c r="CJ40" s="30"/>
-      <c r="CK40" s="31"/>
+      <c r="CH40" s="31"/>
+      <c r="CI40" s="31"/>
+      <c r="CJ40" s="31"/>
+      <c r="CK40" s="32"/>
       <c r="CL40" s="13"/>
       <c r="CM40" s="13"/>
       <c r="CN40" s="2">
@@ -4348,16 +4349,16 @@
       <c r="BX41" s="28"/>
       <c r="BY41" s="29"/>
       <c r="BZ41" s="20"/>
-      <c r="CA41" s="35"/>
-      <c r="CB41" s="32"/>
-      <c r="CC41" s="32"/>
-      <c r="CD41" s="32"/>
-      <c r="CE41" s="33"/>
-      <c r="CG41" s="35"/>
-      <c r="CH41" s="32"/>
-      <c r="CI41" s="32"/>
-      <c r="CJ41" s="32"/>
-      <c r="CK41" s="33"/>
+      <c r="CA41" s="33"/>
+      <c r="CB41" s="34"/>
+      <c r="CC41" s="34"/>
+      <c r="CD41" s="34"/>
+      <c r="CE41" s="35"/>
+      <c r="CG41" s="33"/>
+      <c r="CH41" s="34"/>
+      <c r="CI41" s="34"/>
+      <c r="CJ41" s="34"/>
+      <c r="CK41" s="35"/>
       <c r="CL41" s="13"/>
       <c r="CM41" s="13"/>
       <c r="CN41" s="2">
@@ -4430,42 +4431,42 @@
       <c r="W43" s="12"/>
       <c r="BD43" s="13"/>
       <c r="BF43" s="12"/>
-      <c r="BG43" s="34" t="s">
+      <c r="BG43" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="BH43" s="30"/>
-      <c r="BI43" s="30"/>
-      <c r="BJ43" s="30"/>
-      <c r="BK43" s="30"/>
-      <c r="BL43" s="30"/>
-      <c r="BM43" s="30"/>
-      <c r="BN43" s="30"/>
-      <c r="BO43" s="30"/>
-      <c r="BP43" s="30"/>
-      <c r="BQ43" s="30"/>
-      <c r="BR43" s="30"/>
-      <c r="BS43" s="30"/>
-      <c r="BT43" s="30"/>
-      <c r="BU43" s="30"/>
-      <c r="BV43" s="30"/>
-      <c r="BW43" s="30"/>
-      <c r="BX43" s="30"/>
-      <c r="BY43" s="31"/>
+      <c r="BH43" s="31"/>
+      <c r="BI43" s="31"/>
+      <c r="BJ43" s="31"/>
+      <c r="BK43" s="31"/>
+      <c r="BL43" s="31"/>
+      <c r="BM43" s="31"/>
+      <c r="BN43" s="31"/>
+      <c r="BO43" s="31"/>
+      <c r="BP43" s="31"/>
+      <c r="BQ43" s="31"/>
+      <c r="BR43" s="31"/>
+      <c r="BS43" s="31"/>
+      <c r="BT43" s="31"/>
+      <c r="BU43" s="31"/>
+      <c r="BV43" s="31"/>
+      <c r="BW43" s="31"/>
+      <c r="BX43" s="31"/>
+      <c r="BY43" s="32"/>
       <c r="BZ43" s="20"/>
-      <c r="CA43" s="34" t="s">
+      <c r="CA43" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="CB43" s="30"/>
-      <c r="CC43" s="30"/>
-      <c r="CD43" s="30"/>
-      <c r="CE43" s="31"/>
-      <c r="CG43" s="34" t="s">
+      <c r="CB43" s="31"/>
+      <c r="CC43" s="31"/>
+      <c r="CD43" s="31"/>
+      <c r="CE43" s="32"/>
+      <c r="CG43" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="CH43" s="30"/>
-      <c r="CI43" s="30"/>
-      <c r="CJ43" s="30"/>
-      <c r="CK43" s="31"/>
+      <c r="CH43" s="31"/>
+      <c r="CI43" s="31"/>
+      <c r="CJ43" s="31"/>
+      <c r="CK43" s="32"/>
       <c r="CL43" s="13"/>
       <c r="CM43" s="13"/>
       <c r="CN43" s="2">
@@ -4502,36 +4503,36 @@
       <c r="W44" s="12"/>
       <c r="BD44" s="13"/>
       <c r="BF44" s="12"/>
-      <c r="BG44" s="35"/>
-      <c r="BH44" s="32"/>
-      <c r="BI44" s="32"/>
-      <c r="BJ44" s="32"/>
-      <c r="BK44" s="32"/>
-      <c r="BL44" s="32"/>
-      <c r="BM44" s="32"/>
-      <c r="BN44" s="32"/>
-      <c r="BO44" s="32"/>
-      <c r="BP44" s="32"/>
-      <c r="BQ44" s="32"/>
-      <c r="BR44" s="32"/>
-      <c r="BS44" s="32"/>
-      <c r="BT44" s="32"/>
-      <c r="BU44" s="32"/>
-      <c r="BV44" s="32"/>
-      <c r="BW44" s="32"/>
-      <c r="BX44" s="32"/>
-      <c r="BY44" s="33"/>
+      <c r="BG44" s="33"/>
+      <c r="BH44" s="34"/>
+      <c r="BI44" s="34"/>
+      <c r="BJ44" s="34"/>
+      <c r="BK44" s="34"/>
+      <c r="BL44" s="34"/>
+      <c r="BM44" s="34"/>
+      <c r="BN44" s="34"/>
+      <c r="BO44" s="34"/>
+      <c r="BP44" s="34"/>
+      <c r="BQ44" s="34"/>
+      <c r="BR44" s="34"/>
+      <c r="BS44" s="34"/>
+      <c r="BT44" s="34"/>
+      <c r="BU44" s="34"/>
+      <c r="BV44" s="34"/>
+      <c r="BW44" s="34"/>
+      <c r="BX44" s="34"/>
+      <c r="BY44" s="35"/>
       <c r="BZ44" s="20"/>
-      <c r="CA44" s="35"/>
-      <c r="CB44" s="32"/>
-      <c r="CC44" s="32"/>
-      <c r="CD44" s="32"/>
-      <c r="CE44" s="33"/>
-      <c r="CG44" s="35"/>
-      <c r="CH44" s="32"/>
-      <c r="CI44" s="32"/>
-      <c r="CJ44" s="32"/>
-      <c r="CK44" s="33"/>
+      <c r="CA44" s="33"/>
+      <c r="CB44" s="34"/>
+      <c r="CC44" s="34"/>
+      <c r="CD44" s="34"/>
+      <c r="CE44" s="35"/>
+      <c r="CG44" s="33"/>
+      <c r="CH44" s="34"/>
+      <c r="CI44" s="34"/>
+      <c r="CJ44" s="34"/>
+      <c r="CK44" s="35"/>
       <c r="CL44" s="13"/>
       <c r="CM44" s="13"/>
       <c r="CN44" s="2">
@@ -4616,13 +4617,13 @@
       <c r="BN46" s="25"/>
       <c r="BO46" s="25"/>
       <c r="BP46" s="26"/>
-      <c r="CA46" s="34" t="s">
+      <c r="CA46" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="CB46" s="30"/>
-      <c r="CC46" s="30"/>
-      <c r="CD46" s="30"/>
-      <c r="CE46" s="31"/>
+      <c r="CB46" s="31"/>
+      <c r="CC46" s="31"/>
+      <c r="CD46" s="31"/>
+      <c r="CE46" s="32"/>
       <c r="CG46" s="20"/>
       <c r="CH46" s="20"/>
       <c r="CI46" s="20"/>
@@ -4674,11 +4675,11 @@
       <c r="BN47" s="28"/>
       <c r="BO47" s="28"/>
       <c r="BP47" s="29"/>
-      <c r="CA47" s="35"/>
-      <c r="CB47" s="32"/>
-      <c r="CC47" s="32"/>
-      <c r="CD47" s="32"/>
-      <c r="CE47" s="33"/>
+      <c r="CA47" s="33"/>
+      <c r="CB47" s="34"/>
+      <c r="CC47" s="34"/>
+      <c r="CD47" s="34"/>
+      <c r="CE47" s="35"/>
       <c r="CG47" s="20"/>
       <c r="CH47" s="20"/>
       <c r="CI47" s="20"/>
@@ -4871,27 +4872,24 @@
       <c r="BS50" s="20"/>
       <c r="BT50" s="20"/>
       <c r="BU50" s="20"/>
-      <c r="BV50" s="20"/>
-      <c r="BW50" s="20"/>
-      <c r="BX50" s="20"/>
       <c r="BY50" s="20"/>
       <c r="BZ50" s="20"/>
-      <c r="CA50" s="20"/>
-      <c r="CB50" s="20"/>
-      <c r="CC50" s="20"/>
-      <c r="CD50" s="20"/>
-      <c r="CE50" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="CF50" s="25"/>
-      <c r="CG50" s="26"/>
-      <c r="CH50" s="34" t="s">
+      <c r="CA50" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="CB50" s="31"/>
+      <c r="CC50" s="31"/>
+      <c r="CD50" s="31"/>
+      <c r="CE50" s="31"/>
+      <c r="CF50" s="31"/>
+      <c r="CG50" s="32"/>
+      <c r="CH50" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="CI50" s="30"/>
-      <c r="CJ50" s="30"/>
-      <c r="CK50" s="30"/>
-      <c r="CL50" s="31"/>
+      <c r="CI50" s="31"/>
+      <c r="CJ50" s="31"/>
+      <c r="CK50" s="31"/>
+      <c r="CL50" s="32"/>
       <c r="CM50" s="13"/>
       <c r="CN50" s="2">
         <f t="shared" si="7"/>
@@ -4942,23 +4940,20 @@
       <c r="BS51" s="20"/>
       <c r="BT51" s="20"/>
       <c r="BU51" s="20"/>
-      <c r="BV51" s="20"/>
-      <c r="BW51" s="20"/>
-      <c r="BX51" s="20"/>
       <c r="BY51" s="20"/>
       <c r="BZ51" s="20"/>
-      <c r="CA51" s="20"/>
-      <c r="CB51" s="20"/>
-      <c r="CC51" s="20"/>
-      <c r="CD51" s="20"/>
-      <c r="CE51" s="27"/>
-      <c r="CF51" s="28"/>
-      <c r="CG51" s="29"/>
-      <c r="CH51" s="35"/>
-      <c r="CI51" s="32"/>
-      <c r="CJ51" s="32"/>
-      <c r="CK51" s="32"/>
-      <c r="CL51" s="33"/>
+      <c r="CA51" s="33"/>
+      <c r="CB51" s="34"/>
+      <c r="CC51" s="34"/>
+      <c r="CD51" s="34"/>
+      <c r="CE51" s="34"/>
+      <c r="CF51" s="34"/>
+      <c r="CG51" s="35"/>
+      <c r="CH51" s="33"/>
+      <c r="CI51" s="34"/>
+      <c r="CJ51" s="34"/>
+      <c r="CK51" s="34"/>
+      <c r="CL51" s="35"/>
       <c r="CM51" s="13"/>
       <c r="CN51" s="2">
         <f t="shared" si="7"/>
@@ -5096,13 +5091,13 @@
       <c r="BD54" s="13"/>
       <c r="BF54" s="12"/>
       <c r="CE54" s="11"/>
-      <c r="CG54" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="CH54" s="30"/>
-      <c r="CI54" s="30"/>
-      <c r="CJ54" s="30"/>
-      <c r="CK54" s="31"/>
+      <c r="CG54" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="CH54" s="31"/>
+      <c r="CI54" s="31"/>
+      <c r="CJ54" s="31"/>
+      <c r="CK54" s="32"/>
       <c r="CL54" s="13"/>
       <c r="CM54" s="13"/>
       <c r="CN54" s="2">
@@ -5140,11 +5135,11 @@
       <c r="BD55" s="13"/>
       <c r="BF55" s="12"/>
       <c r="CE55" s="11"/>
-      <c r="CG55" s="35"/>
-      <c r="CH55" s="32"/>
-      <c r="CI55" s="32"/>
-      <c r="CJ55" s="32"/>
-      <c r="CK55" s="33"/>
+      <c r="CG55" s="33"/>
+      <c r="CH55" s="34"/>
+      <c r="CI55" s="34"/>
+      <c r="CJ55" s="34"/>
+      <c r="CK55" s="35"/>
       <c r="CL55" s="13"/>
       <c r="CM55" s="13"/>
       <c r="CN55" s="2">
@@ -5219,13 +5214,13 @@
       <c r="BD57" s="13"/>
       <c r="BF57" s="12"/>
       <c r="CE57" s="11"/>
-      <c r="CG57" s="34" t="s">
+      <c r="CG57" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="CH57" s="30"/>
-      <c r="CI57" s="30"/>
-      <c r="CJ57" s="30"/>
-      <c r="CK57" s="31"/>
+      <c r="CH57" s="31"/>
+      <c r="CI57" s="31"/>
+      <c r="CJ57" s="31"/>
+      <c r="CK57" s="32"/>
       <c r="CL57" s="13"/>
       <c r="CM57" s="13"/>
       <c r="CN57" s="2">
@@ -5263,11 +5258,11 @@
       <c r="BD58" s="13"/>
       <c r="BF58" s="12"/>
       <c r="CE58" s="11"/>
-      <c r="CG58" s="35"/>
-      <c r="CH58" s="32"/>
-      <c r="CI58" s="32"/>
-      <c r="CJ58" s="32"/>
-      <c r="CK58" s="33"/>
+      <c r="CG58" s="33"/>
+      <c r="CH58" s="34"/>
+      <c r="CI58" s="34"/>
+      <c r="CJ58" s="34"/>
+      <c r="CK58" s="35"/>
       <c r="CL58" s="13"/>
       <c r="CM58" s="13"/>
       <c r="CN58" s="2">
@@ -5342,13 +5337,13 @@
       <c r="BD60" s="13"/>
       <c r="BF60" s="12"/>
       <c r="CE60" s="11"/>
-      <c r="CG60" s="34" t="s">
+      <c r="CG60" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="CH60" s="30"/>
-      <c r="CI60" s="30"/>
-      <c r="CJ60" s="30"/>
-      <c r="CK60" s="31"/>
+      <c r="CH60" s="31"/>
+      <c r="CI60" s="31"/>
+      <c r="CJ60" s="31"/>
+      <c r="CK60" s="32"/>
       <c r="CL60" s="13"/>
       <c r="CM60" s="13"/>
       <c r="CN60" s="2">
@@ -5386,11 +5381,11 @@
       <c r="BD61" s="13"/>
       <c r="BF61" s="12"/>
       <c r="CE61" s="11"/>
-      <c r="CG61" s="35"/>
-      <c r="CH61" s="32"/>
-      <c r="CI61" s="32"/>
-      <c r="CJ61" s="32"/>
-      <c r="CK61" s="33"/>
+      <c r="CG61" s="33"/>
+      <c r="CH61" s="34"/>
+      <c r="CI61" s="34"/>
+      <c r="CJ61" s="34"/>
+      <c r="CK61" s="35"/>
       <c r="CL61" s="13"/>
       <c r="CM61" s="13"/>
       <c r="CN61" s="2">
@@ -5465,13 +5460,13 @@
       <c r="BD63" s="13"/>
       <c r="BF63" s="12"/>
       <c r="CE63" s="11"/>
-      <c r="CG63" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="CH63" s="30"/>
-      <c r="CI63" s="30"/>
-      <c r="CJ63" s="30"/>
-      <c r="CK63" s="31"/>
+      <c r="CG63" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="CH63" s="31"/>
+      <c r="CI63" s="31"/>
+      <c r="CJ63" s="31"/>
+      <c r="CK63" s="32"/>
       <c r="CL63" s="13"/>
       <c r="CM63" s="13"/>
       <c r="CN63" s="2">
@@ -5509,11 +5504,11 @@
       <c r="BD64" s="13"/>
       <c r="BF64" s="12"/>
       <c r="CE64" s="11"/>
-      <c r="CG64" s="35"/>
-      <c r="CH64" s="32"/>
-      <c r="CI64" s="32"/>
-      <c r="CJ64" s="32"/>
-      <c r="CK64" s="33"/>
+      <c r="CG64" s="33"/>
+      <c r="CH64" s="34"/>
+      <c r="CI64" s="34"/>
+      <c r="CJ64" s="34"/>
+      <c r="CK64" s="35"/>
       <c r="CL64" s="13"/>
       <c r="CM64" s="13"/>
       <c r="CN64" s="2">
@@ -5588,13 +5583,13 @@
       <c r="BD66" s="13"/>
       <c r="BF66" s="12"/>
       <c r="CE66" s="11"/>
-      <c r="CG66" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="CH66" s="30"/>
-      <c r="CI66" s="30"/>
-      <c r="CJ66" s="30"/>
-      <c r="CK66" s="31"/>
+      <c r="CG66" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="CH66" s="31"/>
+      <c r="CI66" s="31"/>
+      <c r="CJ66" s="31"/>
+      <c r="CK66" s="32"/>
       <c r="CL66" s="13"/>
       <c r="CM66" s="13"/>
       <c r="CN66" s="2">
@@ -5632,11 +5627,11 @@
       <c r="BD67" s="13"/>
       <c r="BF67" s="12"/>
       <c r="CE67" s="11"/>
-      <c r="CG67" s="35"/>
-      <c r="CH67" s="32"/>
-      <c r="CI67" s="32"/>
-      <c r="CJ67" s="32"/>
-      <c r="CK67" s="33"/>
+      <c r="CG67" s="33"/>
+      <c r="CH67" s="34"/>
+      <c r="CI67" s="34"/>
+      <c r="CJ67" s="34"/>
+      <c r="CK67" s="35"/>
       <c r="CL67" s="13"/>
       <c r="CM67" s="13"/>
       <c r="CN67" s="2">
@@ -6541,14 +6536,14 @@
         <v>83</v>
       </c>
       <c r="V90" s="12"/>
-      <c r="W90" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="X90" s="30"/>
-      <c r="Y90" s="30"/>
-      <c r="Z90" s="30"/>
-      <c r="AA90" s="30"/>
-      <c r="AB90" s="31"/>
+      <c r="W90" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="X90" s="31"/>
+      <c r="Y90" s="31"/>
+      <c r="Z90" s="31"/>
+      <c r="AA90" s="31"/>
+      <c r="AB90" s="32"/>
       <c r="CM90" s="13"/>
       <c r="CN90" s="2">
         <f t="shared" si="11"/>
@@ -6581,36 +6576,36 @@
         <v>84</v>
       </c>
       <c r="V91" s="12"/>
-      <c r="W91" s="35"/>
-      <c r="X91" s="32"/>
-      <c r="Y91" s="32"/>
-      <c r="Z91" s="32"/>
-      <c r="AA91" s="32"/>
-      <c r="AB91" s="33"/>
-      <c r="AZ91" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="BA91" s="30"/>
-      <c r="BB91" s="30"/>
-      <c r="BC91" s="30"/>
-      <c r="BD91" s="30"/>
-      <c r="BE91" s="30"/>
-      <c r="BF91" s="30"/>
-      <c r="BG91" s="30"/>
-      <c r="BH91" s="30"/>
-      <c r="BI91" s="31"/>
-      <c r="CC91" s="34" t="s">
+      <c r="W91" s="33"/>
+      <c r="X91" s="34"/>
+      <c r="Y91" s="34"/>
+      <c r="Z91" s="34"/>
+      <c r="AA91" s="34"/>
+      <c r="AB91" s="35"/>
+      <c r="AZ91" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="BA91" s="31"/>
+      <c r="BB91" s="31"/>
+      <c r="BC91" s="31"/>
+      <c r="BD91" s="31"/>
+      <c r="BE91" s="31"/>
+      <c r="BF91" s="31"/>
+      <c r="BG91" s="31"/>
+      <c r="BH91" s="31"/>
+      <c r="BI91" s="32"/>
+      <c r="CC91" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="CD91" s="30"/>
-      <c r="CE91" s="30"/>
-      <c r="CF91" s="30"/>
-      <c r="CG91" s="30"/>
-      <c r="CH91" s="30"/>
-      <c r="CI91" s="30"/>
-      <c r="CJ91" s="30"/>
-      <c r="CK91" s="30"/>
-      <c r="CL91" s="31"/>
+      <c r="CD91" s="31"/>
+      <c r="CE91" s="31"/>
+      <c r="CF91" s="31"/>
+      <c r="CG91" s="31"/>
+      <c r="CH91" s="31"/>
+      <c r="CI91" s="31"/>
+      <c r="CJ91" s="31"/>
+      <c r="CK91" s="31"/>
+      <c r="CL91" s="32"/>
       <c r="CM91" s="13"/>
       <c r="CN91" s="2">
         <f t="shared" si="11"/>
@@ -6747,26 +6742,26 @@
         <v>87</v>
       </c>
       <c r="V94" s="12"/>
-      <c r="AZ94" s="35"/>
-      <c r="BA94" s="32"/>
-      <c r="BB94" s="32"/>
-      <c r="BC94" s="32"/>
-      <c r="BD94" s="32"/>
-      <c r="BE94" s="32"/>
-      <c r="BF94" s="32"/>
-      <c r="BG94" s="32"/>
-      <c r="BH94" s="32"/>
-      <c r="BI94" s="33"/>
-      <c r="CC94" s="35"/>
-      <c r="CD94" s="32"/>
-      <c r="CE94" s="32"/>
-      <c r="CF94" s="32"/>
-      <c r="CG94" s="32"/>
-      <c r="CH94" s="32"/>
-      <c r="CI94" s="32"/>
-      <c r="CJ94" s="32"/>
-      <c r="CK94" s="32"/>
-      <c r="CL94" s="33"/>
+      <c r="AZ94" s="33"/>
+      <c r="BA94" s="34"/>
+      <c r="BB94" s="34"/>
+      <c r="BC94" s="34"/>
+      <c r="BD94" s="34"/>
+      <c r="BE94" s="34"/>
+      <c r="BF94" s="34"/>
+      <c r="BG94" s="34"/>
+      <c r="BH94" s="34"/>
+      <c r="BI94" s="35"/>
+      <c r="CC94" s="33"/>
+      <c r="CD94" s="34"/>
+      <c r="CE94" s="34"/>
+      <c r="CF94" s="34"/>
+      <c r="CG94" s="34"/>
+      <c r="CH94" s="34"/>
+      <c r="CI94" s="34"/>
+      <c r="CJ94" s="34"/>
+      <c r="CK94" s="34"/>
+      <c r="CL94" s="35"/>
       <c r="CM94" s="13"/>
       <c r="CN94" s="2">
         <f t="shared" si="11"/>
@@ -8494,40 +8489,10 @@
       <c r="DH112" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="BG46:BP47"/>
-    <mergeCell ref="BG40:BY41"/>
-    <mergeCell ref="BG43:BY44"/>
-    <mergeCell ref="W90:AB91"/>
-    <mergeCell ref="BY31:CK33"/>
-    <mergeCell ref="CC91:CL94"/>
-    <mergeCell ref="AZ91:BI94"/>
-    <mergeCell ref="CA40:CE41"/>
-    <mergeCell ref="CA43:CE44"/>
-    <mergeCell ref="CA46:CE47"/>
-    <mergeCell ref="CG40:CK41"/>
-    <mergeCell ref="CG43:CK44"/>
-    <mergeCell ref="CG66:CK67"/>
-    <mergeCell ref="CH50:CL51"/>
-    <mergeCell ref="CE50:CG51"/>
-    <mergeCell ref="CG54:CK55"/>
-    <mergeCell ref="CG57:CK58"/>
-    <mergeCell ref="CG60:CK61"/>
-    <mergeCell ref="CG63:CK64"/>
-    <mergeCell ref="AP25:BU26"/>
-    <mergeCell ref="AP28:AY29"/>
-    <mergeCell ref="BY22:CB23"/>
-    <mergeCell ref="CJ22:CK23"/>
-    <mergeCell ref="CF22:CG23"/>
-    <mergeCell ref="BY28:CD29"/>
-    <mergeCell ref="CF28:CK29"/>
-    <mergeCell ref="AB22:AL23"/>
-    <mergeCell ref="X25:AA26"/>
-    <mergeCell ref="X28:AA29"/>
-    <mergeCell ref="X31:AA32"/>
-    <mergeCell ref="AB25:AL26"/>
-    <mergeCell ref="AB28:AL29"/>
-    <mergeCell ref="AB31:AL32"/>
+  <mergeCells count="51">
+    <mergeCell ref="BR18:BV19"/>
+    <mergeCell ref="BL18:BQ19"/>
+    <mergeCell ref="CA50:CG51"/>
     <mergeCell ref="W18:AF19"/>
     <mergeCell ref="AO18:AX19"/>
     <mergeCell ref="BX18:CG19"/>
@@ -8544,6 +8509,38 @@
     <mergeCell ref="AT36:AV37"/>
     <mergeCell ref="AP36:AQ37"/>
     <mergeCell ref="X22:AA23"/>
+    <mergeCell ref="AB22:AL23"/>
+    <mergeCell ref="X25:AA26"/>
+    <mergeCell ref="X28:AA29"/>
+    <mergeCell ref="X31:AA32"/>
+    <mergeCell ref="AB25:AL26"/>
+    <mergeCell ref="AB28:AL29"/>
+    <mergeCell ref="AB31:AL32"/>
+    <mergeCell ref="BY22:CB23"/>
+    <mergeCell ref="CJ22:CK23"/>
+    <mergeCell ref="CF22:CG23"/>
+    <mergeCell ref="BY28:CD29"/>
+    <mergeCell ref="CF28:CK29"/>
+    <mergeCell ref="CG57:CK58"/>
+    <mergeCell ref="CG60:CK61"/>
+    <mergeCell ref="CG63:CK64"/>
+    <mergeCell ref="AP25:BU26"/>
+    <mergeCell ref="AP28:AY29"/>
+    <mergeCell ref="BG46:BP47"/>
+    <mergeCell ref="BG40:BY41"/>
+    <mergeCell ref="BG43:BY44"/>
+    <mergeCell ref="W90:AB91"/>
+    <mergeCell ref="BY31:CK33"/>
+    <mergeCell ref="CC91:CL94"/>
+    <mergeCell ref="AZ91:BI94"/>
+    <mergeCell ref="CA40:CE41"/>
+    <mergeCell ref="CA43:CE44"/>
+    <mergeCell ref="CA46:CE47"/>
+    <mergeCell ref="CG40:CK41"/>
+    <mergeCell ref="CG43:CK44"/>
+    <mergeCell ref="CG66:CK67"/>
+    <mergeCell ref="CH50:CL51"/>
+    <mergeCell ref="CG54:CK55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Layout.xlsx with revised document structure
</commit_message>
<xml_diff>
--- a/doc/Layout.xlsx
+++ b/doc/Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Arma 3 Modding\21_ZeusJukebox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA780D5D-3559-45B7-B783-229FA0D7AEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E9AB3D-16B1-4F79-9A2A-A397C469B777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{682E6184-E15B-4402-836A-91257A3551C0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>*</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>(un) favorite Song</t>
-  </si>
-  <si>
-    <t>Zeus Jukebox Logs</t>
   </si>
   <si>
     <t>Autoplay Preview:</t>
@@ -385,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -457,6 +454,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -474,24 +489,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -500,6 +497,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5B835F-835A-4242-BD99-7FE00DEEB233}">
   <dimension ref="A1:DH112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="CV49" sqref="CV49"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CC72" sqref="CC72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.140625" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2540,18 +2540,18 @@
         <v>11</v>
       </c>
       <c r="V18" s="12"/>
-      <c r="W18" s="24" t="s">
+      <c r="W18" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="X18" s="25"/>
-      <c r="Y18" s="25"/>
-      <c r="Z18" s="25"/>
-      <c r="AA18" s="25"/>
-      <c r="AB18" s="25"/>
-      <c r="AC18" s="25"/>
-      <c r="AD18" s="25"/>
-      <c r="AE18" s="25"/>
-      <c r="AF18" s="26"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="31"/>
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="32"/>
       <c r="AG18" s="20"/>
       <c r="AH18" s="20"/>
       <c r="AI18" s="20"/>
@@ -2559,18 +2559,18 @@
       <c r="AK18" s="20"/>
       <c r="AL18" s="20"/>
       <c r="AM18" s="20"/>
-      <c r="AO18" s="24" t="s">
+      <c r="AO18" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="AP18" s="25"/>
-      <c r="AQ18" s="25"/>
-      <c r="AR18" s="25"/>
-      <c r="AS18" s="25"/>
-      <c r="AT18" s="25"/>
-      <c r="AU18" s="25"/>
-      <c r="AV18" s="25"/>
-      <c r="AW18" s="25"/>
-      <c r="AX18" s="26"/>
+      <c r="AP18" s="31"/>
+      <c r="AQ18" s="31"/>
+      <c r="AR18" s="31"/>
+      <c r="AS18" s="31"/>
+      <c r="AT18" s="31"/>
+      <c r="AU18" s="31"/>
+      <c r="AV18" s="31"/>
+      <c r="AW18" s="31"/>
+      <c r="AX18" s="32"/>
       <c r="AY18" s="20"/>
       <c r="AZ18" s="20"/>
       <c r="BA18" s="20"/>
@@ -2581,33 +2581,33 @@
       <c r="BF18" s="20"/>
       <c r="BG18" s="20"/>
       <c r="BK18" s="20"/>
-      <c r="BL18" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="BM18" s="31"/>
-      <c r="BN18" s="31"/>
-      <c r="BO18" s="31"/>
-      <c r="BP18" s="31"/>
-      <c r="BQ18" s="32"/>
-      <c r="BR18" s="30" t="s">
+      <c r="BL18" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="BM18" s="25"/>
+      <c r="BN18" s="25"/>
+      <c r="BO18" s="25"/>
+      <c r="BP18" s="25"/>
+      <c r="BQ18" s="26"/>
+      <c r="BR18" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="BS18" s="31"/>
-      <c r="BT18" s="31"/>
-      <c r="BU18" s="31"/>
-      <c r="BV18" s="32"/>
-      <c r="BX18" s="24" t="s">
+      <c r="BS18" s="25"/>
+      <c r="BT18" s="25"/>
+      <c r="BU18" s="25"/>
+      <c r="BV18" s="26"/>
+      <c r="BX18" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="BY18" s="25"/>
-      <c r="BZ18" s="25"/>
-      <c r="CA18" s="25"/>
-      <c r="CB18" s="25"/>
-      <c r="CC18" s="25"/>
-      <c r="CD18" s="25"/>
-      <c r="CE18" s="25"/>
-      <c r="CF18" s="25"/>
-      <c r="CG18" s="26"/>
+      <c r="BY18" s="31"/>
+      <c r="BZ18" s="31"/>
+      <c r="CA18" s="31"/>
+      <c r="CB18" s="31"/>
+      <c r="CC18" s="31"/>
+      <c r="CD18" s="31"/>
+      <c r="CE18" s="31"/>
+      <c r="CF18" s="31"/>
+      <c r="CG18" s="32"/>
       <c r="CH18" s="20"/>
       <c r="CI18" s="20"/>
       <c r="CJ18" s="20"/>
@@ -2645,16 +2645,16 @@
         <v>12</v>
       </c>
       <c r="V19" s="12"/>
-      <c r="W19" s="27"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="28"/>
-      <c r="AE19" s="28"/>
-      <c r="AF19" s="29"/>
+      <c r="W19" s="33"/>
+      <c r="X19" s="34"/>
+      <c r="Y19" s="34"/>
+      <c r="Z19" s="34"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="34"/>
+      <c r="AC19" s="34"/>
+      <c r="AD19" s="34"/>
+      <c r="AE19" s="34"/>
+      <c r="AF19" s="35"/>
       <c r="AG19" s="20"/>
       <c r="AH19" s="20"/>
       <c r="AI19" s="20"/>
@@ -2662,16 +2662,16 @@
       <c r="AK19" s="20"/>
       <c r="AL19" s="20"/>
       <c r="AM19" s="20"/>
-      <c r="AO19" s="27"/>
-      <c r="AP19" s="28"/>
-      <c r="AQ19" s="28"/>
-      <c r="AR19" s="28"/>
-      <c r="AS19" s="28"/>
-      <c r="AT19" s="28"/>
-      <c r="AU19" s="28"/>
-      <c r="AV19" s="28"/>
-      <c r="AW19" s="28"/>
-      <c r="AX19" s="29"/>
+      <c r="AO19" s="33"/>
+      <c r="AP19" s="34"/>
+      <c r="AQ19" s="34"/>
+      <c r="AR19" s="34"/>
+      <c r="AS19" s="34"/>
+      <c r="AT19" s="34"/>
+      <c r="AU19" s="34"/>
+      <c r="AV19" s="34"/>
+      <c r="AW19" s="34"/>
+      <c r="AX19" s="35"/>
       <c r="AY19" s="20"/>
       <c r="AZ19" s="20"/>
       <c r="BA19" s="20"/>
@@ -2682,27 +2682,27 @@
       <c r="BF19" s="20"/>
       <c r="BG19" s="20"/>
       <c r="BK19" s="20"/>
-      <c r="BL19" s="33"/>
-      <c r="BM19" s="34"/>
-      <c r="BN19" s="34"/>
-      <c r="BO19" s="34"/>
-      <c r="BP19" s="34"/>
-      <c r="BQ19" s="35"/>
-      <c r="BR19" s="33"/>
-      <c r="BS19" s="34"/>
-      <c r="BT19" s="34"/>
-      <c r="BU19" s="34"/>
-      <c r="BV19" s="35"/>
-      <c r="BX19" s="27"/>
-      <c r="BY19" s="28"/>
-      <c r="BZ19" s="28"/>
-      <c r="CA19" s="28"/>
-      <c r="CB19" s="28"/>
-      <c r="CC19" s="28"/>
-      <c r="CD19" s="28"/>
-      <c r="CE19" s="28"/>
-      <c r="CF19" s="28"/>
-      <c r="CG19" s="29"/>
+      <c r="BL19" s="27"/>
+      <c r="BM19" s="28"/>
+      <c r="BN19" s="28"/>
+      <c r="BO19" s="28"/>
+      <c r="BP19" s="28"/>
+      <c r="BQ19" s="29"/>
+      <c r="BR19" s="27"/>
+      <c r="BS19" s="28"/>
+      <c r="BT19" s="28"/>
+      <c r="BU19" s="28"/>
+      <c r="BV19" s="29"/>
+      <c r="BX19" s="33"/>
+      <c r="BY19" s="34"/>
+      <c r="BZ19" s="34"/>
+      <c r="CA19" s="34"/>
+      <c r="CB19" s="34"/>
+      <c r="CC19" s="34"/>
+      <c r="CD19" s="34"/>
+      <c r="CE19" s="34"/>
+      <c r="CF19" s="34"/>
+      <c r="CG19" s="35"/>
       <c r="CH19" s="20"/>
       <c r="CI19" s="20"/>
       <c r="CJ19" s="20"/>
@@ -2871,64 +2871,64 @@
       </c>
       <c r="V22" s="12"/>
       <c r="W22" s="12"/>
-      <c r="X22" s="24" t="s">
+      <c r="X22" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="Y22" s="25"/>
-      <c r="Z22" s="25"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="24" t="s">
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="32"/>
+      <c r="AB22" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AC22" s="25"/>
-      <c r="AD22" s="25"/>
-      <c r="AE22" s="25"/>
-      <c r="AF22" s="25"/>
-      <c r="AG22" s="25"/>
-      <c r="AH22" s="25"/>
-      <c r="AI22" s="25"/>
-      <c r="AJ22" s="25"/>
-      <c r="AK22" s="25"/>
-      <c r="AL22" s="26"/>
+      <c r="AC22" s="31"/>
+      <c r="AD22" s="31"/>
+      <c r="AE22" s="31"/>
+      <c r="AF22" s="31"/>
+      <c r="AG22" s="31"/>
+      <c r="AH22" s="31"/>
+      <c r="AI22" s="31"/>
+      <c r="AJ22" s="31"/>
+      <c r="AK22" s="31"/>
+      <c r="AL22" s="32"/>
       <c r="AM22" s="13"/>
       <c r="AO22" s="12"/>
-      <c r="AP22" s="24" t="s">
+      <c r="AP22" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="AQ22" s="25"/>
-      <c r="AR22" s="25"/>
-      <c r="AS22" s="25"/>
-      <c r="AT22" s="25"/>
-      <c r="AU22" s="25"/>
-      <c r="AV22" s="25"/>
-      <c r="AW22" s="25"/>
-      <c r="AX22" s="25"/>
-      <c r="AY22" s="25"/>
-      <c r="AZ22" s="25"/>
-      <c r="BA22" s="25"/>
-      <c r="BB22" s="25"/>
-      <c r="BC22" s="25"/>
-      <c r="BD22" s="25"/>
-      <c r="BE22" s="25"/>
-      <c r="BF22" s="25"/>
-      <c r="BG22" s="25"/>
-      <c r="BH22" s="26"/>
+      <c r="AQ22" s="31"/>
+      <c r="AR22" s="31"/>
+      <c r="AS22" s="31"/>
+      <c r="AT22" s="31"/>
+      <c r="AU22" s="31"/>
+      <c r="AV22" s="31"/>
+      <c r="AW22" s="31"/>
+      <c r="AX22" s="31"/>
+      <c r="AY22" s="31"/>
+      <c r="AZ22" s="31"/>
+      <c r="BA22" s="31"/>
+      <c r="BB22" s="31"/>
+      <c r="BC22" s="31"/>
+      <c r="BD22" s="31"/>
+      <c r="BE22" s="31"/>
+      <c r="BF22" s="31"/>
+      <c r="BG22" s="31"/>
+      <c r="BH22" s="32"/>
       <c r="BV22" s="13"/>
       <c r="BX22" s="12"/>
-      <c r="BY22" s="24" t="s">
+      <c r="BY22" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="BZ22" s="25"/>
-      <c r="CA22" s="25"/>
-      <c r="CB22" s="26"/>
-      <c r="CF22" s="30" t="s">
+      <c r="BZ22" s="31"/>
+      <c r="CA22" s="31"/>
+      <c r="CB22" s="32"/>
+      <c r="CF22" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="CG22" s="32"/>
-      <c r="CJ22" s="30" t="s">
+      <c r="CG22" s="26"/>
+      <c r="CJ22" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="CK22" s="32"/>
+      <c r="CK22" s="26"/>
       <c r="CL22" s="13"/>
       <c r="CM22" s="13"/>
       <c r="CN22" s="2">
@@ -2963,52 +2963,52 @@
       </c>
       <c r="V23" s="12"/>
       <c r="W23" s="12"/>
-      <c r="X23" s="27"/>
-      <c r="Y23" s="28"/>
-      <c r="Z23" s="28"/>
-      <c r="AA23" s="29"/>
-      <c r="AB23" s="27"/>
-      <c r="AC23" s="28"/>
-      <c r="AD23" s="28"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
-      <c r="AG23" s="28"/>
-      <c r="AH23" s="28"/>
-      <c r="AI23" s="28"/>
-      <c r="AJ23" s="28"/>
-      <c r="AK23" s="28"/>
-      <c r="AL23" s="29"/>
+      <c r="X23" s="33"/>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="34"/>
+      <c r="AA23" s="35"/>
+      <c r="AB23" s="33"/>
+      <c r="AC23" s="34"/>
+      <c r="AD23" s="34"/>
+      <c r="AE23" s="34"/>
+      <c r="AF23" s="34"/>
+      <c r="AG23" s="34"/>
+      <c r="AH23" s="34"/>
+      <c r="AI23" s="34"/>
+      <c r="AJ23" s="34"/>
+      <c r="AK23" s="34"/>
+      <c r="AL23" s="35"/>
       <c r="AM23" s="13"/>
       <c r="AO23" s="12"/>
-      <c r="AP23" s="27"/>
-      <c r="AQ23" s="28"/>
-      <c r="AR23" s="28"/>
-      <c r="AS23" s="28"/>
-      <c r="AT23" s="28"/>
-      <c r="AU23" s="28"/>
-      <c r="AV23" s="28"/>
-      <c r="AW23" s="28"/>
-      <c r="AX23" s="28"/>
-      <c r="AY23" s="28"/>
-      <c r="AZ23" s="28"/>
-      <c r="BA23" s="28"/>
-      <c r="BB23" s="28"/>
-      <c r="BC23" s="28"/>
-      <c r="BD23" s="28"/>
-      <c r="BE23" s="28"/>
-      <c r="BF23" s="28"/>
-      <c r="BG23" s="28"/>
-      <c r="BH23" s="29"/>
+      <c r="AP23" s="33"/>
+      <c r="AQ23" s="34"/>
+      <c r="AR23" s="34"/>
+      <c r="AS23" s="34"/>
+      <c r="AT23" s="34"/>
+      <c r="AU23" s="34"/>
+      <c r="AV23" s="34"/>
+      <c r="AW23" s="34"/>
+      <c r="AX23" s="34"/>
+      <c r="AY23" s="34"/>
+      <c r="AZ23" s="34"/>
+      <c r="BA23" s="34"/>
+      <c r="BB23" s="34"/>
+      <c r="BC23" s="34"/>
+      <c r="BD23" s="34"/>
+      <c r="BE23" s="34"/>
+      <c r="BF23" s="34"/>
+      <c r="BG23" s="34"/>
+      <c r="BH23" s="35"/>
       <c r="BV23" s="13"/>
       <c r="BX23" s="12"/>
-      <c r="BY23" s="27"/>
-      <c r="BZ23" s="28"/>
-      <c r="CA23" s="28"/>
-      <c r="CB23" s="29"/>
-      <c r="CF23" s="33"/>
-      <c r="CG23" s="35"/>
-      <c r="CJ23" s="33"/>
-      <c r="CK23" s="35"/>
+      <c r="BY23" s="33"/>
+      <c r="BZ23" s="34"/>
+      <c r="CA23" s="34"/>
+      <c r="CB23" s="35"/>
+      <c r="CF23" s="27"/>
+      <c r="CG23" s="29"/>
+      <c r="CJ23" s="27"/>
+      <c r="CK23" s="29"/>
       <c r="CL23" s="13"/>
       <c r="CM23" s="13"/>
       <c r="CN23" s="2">
@@ -3081,61 +3081,61 @@
       </c>
       <c r="V25" s="12"/>
       <c r="W25" s="12"/>
-      <c r="X25" s="24" t="s">
+      <c r="X25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="Y25" s="25"/>
-      <c r="Z25" s="25"/>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="24" t="s">
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="31"/>
+      <c r="AA25" s="32"/>
+      <c r="AB25" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AC25" s="25"/>
-      <c r="AD25" s="25"/>
-      <c r="AE25" s="25"/>
-      <c r="AF25" s="25"/>
-      <c r="AG25" s="25"/>
-      <c r="AH25" s="25"/>
-      <c r="AI25" s="25"/>
-      <c r="AJ25" s="25"/>
-      <c r="AK25" s="25"/>
-      <c r="AL25" s="26"/>
+      <c r="AC25" s="31"/>
+      <c r="AD25" s="31"/>
+      <c r="AE25" s="31"/>
+      <c r="AF25" s="31"/>
+      <c r="AG25" s="31"/>
+      <c r="AH25" s="31"/>
+      <c r="AI25" s="31"/>
+      <c r="AJ25" s="31"/>
+      <c r="AK25" s="31"/>
+      <c r="AL25" s="32"/>
       <c r="AM25" s="13"/>
       <c r="AO25" s="12"/>
-      <c r="AP25" s="30" t="s">
+      <c r="AP25" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AQ25" s="31"/>
-      <c r="AR25" s="31"/>
-      <c r="AS25" s="31"/>
-      <c r="AT25" s="31"/>
-      <c r="AU25" s="31"/>
-      <c r="AV25" s="31"/>
-      <c r="AW25" s="31"/>
-      <c r="AX25" s="31"/>
-      <c r="AY25" s="31"/>
-      <c r="AZ25" s="31"/>
-      <c r="BA25" s="31"/>
-      <c r="BB25" s="31"/>
-      <c r="BC25" s="31"/>
-      <c r="BD25" s="31"/>
-      <c r="BE25" s="31"/>
-      <c r="BF25" s="31"/>
-      <c r="BG25" s="31"/>
-      <c r="BH25" s="31"/>
-      <c r="BI25" s="31"/>
-      <c r="BJ25" s="31"/>
-      <c r="BK25" s="31"/>
-      <c r="BL25" s="31"/>
-      <c r="BM25" s="31"/>
-      <c r="BN25" s="31"/>
-      <c r="BO25" s="31"/>
-      <c r="BP25" s="31"/>
-      <c r="BQ25" s="31"/>
-      <c r="BR25" s="31"/>
-      <c r="BS25" s="31"/>
-      <c r="BT25" s="31"/>
-      <c r="BU25" s="32"/>
+      <c r="AQ25" s="25"/>
+      <c r="AR25" s="25"/>
+      <c r="AS25" s="25"/>
+      <c r="AT25" s="25"/>
+      <c r="AU25" s="25"/>
+      <c r="AV25" s="25"/>
+      <c r="AW25" s="25"/>
+      <c r="AX25" s="25"/>
+      <c r="AY25" s="25"/>
+      <c r="AZ25" s="25"/>
+      <c r="BA25" s="25"/>
+      <c r="BB25" s="25"/>
+      <c r="BC25" s="25"/>
+      <c r="BD25" s="25"/>
+      <c r="BE25" s="25"/>
+      <c r="BF25" s="25"/>
+      <c r="BG25" s="25"/>
+      <c r="BH25" s="25"/>
+      <c r="BI25" s="25"/>
+      <c r="BJ25" s="25"/>
+      <c r="BK25" s="25"/>
+      <c r="BL25" s="25"/>
+      <c r="BM25" s="25"/>
+      <c r="BN25" s="25"/>
+      <c r="BO25" s="25"/>
+      <c r="BP25" s="25"/>
+      <c r="BQ25" s="25"/>
+      <c r="BR25" s="25"/>
+      <c r="BS25" s="25"/>
+      <c r="BT25" s="25"/>
+      <c r="BU25" s="26"/>
       <c r="BV25" s="13"/>
       <c r="BX25" s="12"/>
       <c r="CL25" s="13"/>
@@ -3172,55 +3172,55 @@
       </c>
       <c r="V26" s="12"/>
       <c r="W26" s="12"/>
-      <c r="X26" s="27"/>
-      <c r="Y26" s="28"/>
-      <c r="Z26" s="28"/>
-      <c r="AA26" s="29"/>
-      <c r="AB26" s="27"/>
-      <c r="AC26" s="28"/>
-      <c r="AD26" s="28"/>
-      <c r="AE26" s="28"/>
-      <c r="AF26" s="28"/>
-      <c r="AG26" s="28"/>
-      <c r="AH26" s="28"/>
-      <c r="AI26" s="28"/>
-      <c r="AJ26" s="28"/>
-      <c r="AK26" s="28"/>
-      <c r="AL26" s="29"/>
+      <c r="X26" s="33"/>
+      <c r="Y26" s="34"/>
+      <c r="Z26" s="34"/>
+      <c r="AA26" s="35"/>
+      <c r="AB26" s="33"/>
+      <c r="AC26" s="34"/>
+      <c r="AD26" s="34"/>
+      <c r="AE26" s="34"/>
+      <c r="AF26" s="34"/>
+      <c r="AG26" s="34"/>
+      <c r="AH26" s="34"/>
+      <c r="AI26" s="34"/>
+      <c r="AJ26" s="34"/>
+      <c r="AK26" s="34"/>
+      <c r="AL26" s="35"/>
       <c r="AM26" s="13"/>
       <c r="AO26" s="12"/>
-      <c r="AP26" s="33"/>
-      <c r="AQ26" s="34"/>
-      <c r="AR26" s="34"/>
-      <c r="AS26" s="34"/>
-      <c r="AT26" s="34"/>
-      <c r="AU26" s="34"/>
-      <c r="AV26" s="34"/>
-      <c r="AW26" s="34"/>
-      <c r="AX26" s="34"/>
-      <c r="AY26" s="34"/>
-      <c r="AZ26" s="34"/>
-      <c r="BA26" s="34"/>
-      <c r="BB26" s="34"/>
-      <c r="BC26" s="34"/>
-      <c r="BD26" s="34"/>
-      <c r="BE26" s="34"/>
-      <c r="BF26" s="34"/>
-      <c r="BG26" s="34"/>
-      <c r="BH26" s="34"/>
-      <c r="BI26" s="34"/>
-      <c r="BJ26" s="34"/>
-      <c r="BK26" s="34"/>
-      <c r="BL26" s="34"/>
-      <c r="BM26" s="34"/>
-      <c r="BN26" s="34"/>
-      <c r="BO26" s="34"/>
-      <c r="BP26" s="34"/>
-      <c r="BQ26" s="34"/>
-      <c r="BR26" s="34"/>
-      <c r="BS26" s="34"/>
-      <c r="BT26" s="34"/>
-      <c r="BU26" s="35"/>
+      <c r="AP26" s="27"/>
+      <c r="AQ26" s="28"/>
+      <c r="AR26" s="28"/>
+      <c r="AS26" s="28"/>
+      <c r="AT26" s="28"/>
+      <c r="AU26" s="28"/>
+      <c r="AV26" s="28"/>
+      <c r="AW26" s="28"/>
+      <c r="AX26" s="28"/>
+      <c r="AY26" s="28"/>
+      <c r="AZ26" s="28"/>
+      <c r="BA26" s="28"/>
+      <c r="BB26" s="28"/>
+      <c r="BC26" s="28"/>
+      <c r="BD26" s="28"/>
+      <c r="BE26" s="28"/>
+      <c r="BF26" s="28"/>
+      <c r="BG26" s="28"/>
+      <c r="BH26" s="28"/>
+      <c r="BI26" s="28"/>
+      <c r="BJ26" s="28"/>
+      <c r="BK26" s="28"/>
+      <c r="BL26" s="28"/>
+      <c r="BM26" s="28"/>
+      <c r="BN26" s="28"/>
+      <c r="BO26" s="28"/>
+      <c r="BP26" s="28"/>
+      <c r="BQ26" s="28"/>
+      <c r="BR26" s="28"/>
+      <c r="BS26" s="28"/>
+      <c r="BT26" s="28"/>
+      <c r="BU26" s="29"/>
       <c r="BV26" s="13"/>
       <c r="BX26" s="12"/>
       <c r="CL26" s="13"/>
@@ -3295,39 +3295,39 @@
       </c>
       <c r="V28" s="12"/>
       <c r="W28" s="12"/>
-      <c r="X28" s="24" t="s">
+      <c r="X28" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="25"/>
-      <c r="AA28" s="26"/>
-      <c r="AB28" s="24" t="s">
+      <c r="Y28" s="31"/>
+      <c r="Z28" s="31"/>
+      <c r="AA28" s="32"/>
+      <c r="AB28" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AC28" s="25"/>
-      <c r="AD28" s="25"/>
-      <c r="AE28" s="25"/>
-      <c r="AF28" s="25"/>
-      <c r="AG28" s="25"/>
-      <c r="AH28" s="25"/>
-      <c r="AI28" s="25"/>
-      <c r="AJ28" s="25"/>
-      <c r="AK28" s="25"/>
-      <c r="AL28" s="26"/>
+      <c r="AC28" s="31"/>
+      <c r="AD28" s="31"/>
+      <c r="AE28" s="31"/>
+      <c r="AF28" s="31"/>
+      <c r="AG28" s="31"/>
+      <c r="AH28" s="31"/>
+      <c r="AI28" s="31"/>
+      <c r="AJ28" s="31"/>
+      <c r="AK28" s="31"/>
+      <c r="AL28" s="32"/>
       <c r="AM28" s="13"/>
       <c r="AO28" s="12"/>
-      <c r="AP28" s="24" t="s">
+      <c r="AP28" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="AQ28" s="25"/>
-      <c r="AR28" s="25"/>
-      <c r="AS28" s="25"/>
-      <c r="AT28" s="25"/>
-      <c r="AU28" s="25"/>
-      <c r="AV28" s="25"/>
-      <c r="AW28" s="25"/>
-      <c r="AX28" s="25"/>
-      <c r="AY28" s="26"/>
+      <c r="AQ28" s="31"/>
+      <c r="AR28" s="31"/>
+      <c r="AS28" s="31"/>
+      <c r="AT28" s="31"/>
+      <c r="AU28" s="31"/>
+      <c r="AV28" s="31"/>
+      <c r="AW28" s="31"/>
+      <c r="AX28" s="31"/>
+      <c r="AY28" s="32"/>
       <c r="AZ28" s="20"/>
       <c r="BB28" s="20"/>
       <c r="BC28" s="20"/>
@@ -3343,22 +3343,22 @@
       <c r="BN28" s="20"/>
       <c r="BV28" s="13"/>
       <c r="BX28" s="12"/>
-      <c r="BY28" s="30" t="s">
+      <c r="BY28" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="BZ28" s="31"/>
-      <c r="CA28" s="31"/>
-      <c r="CB28" s="31"/>
-      <c r="CC28" s="31"/>
-      <c r="CD28" s="32"/>
-      <c r="CF28" s="30" t="s">
+      <c r="BZ28" s="25"/>
+      <c r="CA28" s="25"/>
+      <c r="CB28" s="25"/>
+      <c r="CC28" s="25"/>
+      <c r="CD28" s="26"/>
+      <c r="CF28" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="CG28" s="31"/>
-      <c r="CH28" s="31"/>
-      <c r="CI28" s="31"/>
-      <c r="CJ28" s="31"/>
-      <c r="CK28" s="32"/>
+      <c r="CG28" s="25"/>
+      <c r="CH28" s="25"/>
+      <c r="CI28" s="25"/>
+      <c r="CJ28" s="25"/>
+      <c r="CK28" s="26"/>
       <c r="CL28" s="13"/>
       <c r="CM28" s="13"/>
       <c r="CN28" s="2">
@@ -3393,33 +3393,33 @@
       </c>
       <c r="V29" s="12"/>
       <c r="W29" s="12"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="28"/>
-      <c r="Z29" s="28"/>
-      <c r="AA29" s="29"/>
-      <c r="AB29" s="27"/>
-      <c r="AC29" s="28"/>
-      <c r="AD29" s="28"/>
-      <c r="AE29" s="28"/>
-      <c r="AF29" s="28"/>
-      <c r="AG29" s="28"/>
-      <c r="AH29" s="28"/>
-      <c r="AI29" s="28"/>
-      <c r="AJ29" s="28"/>
-      <c r="AK29" s="28"/>
-      <c r="AL29" s="29"/>
+      <c r="X29" s="33"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="34"/>
+      <c r="AA29" s="35"/>
+      <c r="AB29" s="33"/>
+      <c r="AC29" s="34"/>
+      <c r="AD29" s="34"/>
+      <c r="AE29" s="34"/>
+      <c r="AF29" s="34"/>
+      <c r="AG29" s="34"/>
+      <c r="AH29" s="34"/>
+      <c r="AI29" s="34"/>
+      <c r="AJ29" s="34"/>
+      <c r="AK29" s="34"/>
+      <c r="AL29" s="35"/>
       <c r="AM29" s="13"/>
       <c r="AO29" s="12"/>
-      <c r="AP29" s="27"/>
-      <c r="AQ29" s="28"/>
-      <c r="AR29" s="28"/>
-      <c r="AS29" s="28"/>
-      <c r="AT29" s="28"/>
-      <c r="AU29" s="28"/>
-      <c r="AV29" s="28"/>
-      <c r="AW29" s="28"/>
-      <c r="AX29" s="28"/>
-      <c r="AY29" s="29"/>
+      <c r="AP29" s="33"/>
+      <c r="AQ29" s="34"/>
+      <c r="AR29" s="34"/>
+      <c r="AS29" s="34"/>
+      <c r="AT29" s="34"/>
+      <c r="AU29" s="34"/>
+      <c r="AV29" s="34"/>
+      <c r="AW29" s="34"/>
+      <c r="AX29" s="34"/>
+      <c r="AY29" s="35"/>
       <c r="AZ29" s="20"/>
       <c r="BB29" s="20"/>
       <c r="BC29" s="20"/>
@@ -3435,18 +3435,18 @@
       <c r="BN29" s="20"/>
       <c r="BV29" s="13"/>
       <c r="BX29" s="12"/>
-      <c r="BY29" s="33"/>
-      <c r="BZ29" s="34"/>
-      <c r="CA29" s="34"/>
-      <c r="CB29" s="34"/>
-      <c r="CC29" s="34"/>
-      <c r="CD29" s="35"/>
-      <c r="CF29" s="33"/>
-      <c r="CG29" s="34"/>
-      <c r="CH29" s="34"/>
-      <c r="CI29" s="34"/>
-      <c r="CJ29" s="34"/>
-      <c r="CK29" s="35"/>
+      <c r="BY29" s="27"/>
+      <c r="BZ29" s="28"/>
+      <c r="CA29" s="28"/>
+      <c r="CB29" s="28"/>
+      <c r="CC29" s="28"/>
+      <c r="CD29" s="29"/>
+      <c r="CF29" s="27"/>
+      <c r="CG29" s="28"/>
+      <c r="CH29" s="28"/>
+      <c r="CI29" s="28"/>
+      <c r="CJ29" s="28"/>
+      <c r="CK29" s="29"/>
       <c r="CL29" s="13"/>
       <c r="CM29" s="13"/>
       <c r="CN29" s="2">
@@ -3537,76 +3537,76 @@
       </c>
       <c r="V31" s="12"/>
       <c r="W31" s="12"/>
-      <c r="X31" s="24" t="s">
+      <c r="X31" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Y31" s="25"/>
-      <c r="Z31" s="25"/>
-      <c r="AA31" s="26"/>
-      <c r="AB31" s="24" t="s">
+      <c r="Y31" s="31"/>
+      <c r="Z31" s="31"/>
+      <c r="AA31" s="32"/>
+      <c r="AB31" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AC31" s="25"/>
-      <c r="AD31" s="25"/>
-      <c r="AE31" s="25"/>
-      <c r="AF31" s="25"/>
-      <c r="AG31" s="25"/>
-      <c r="AH31" s="25"/>
-      <c r="AI31" s="25"/>
-      <c r="AJ31" s="25"/>
-      <c r="AK31" s="25"/>
-      <c r="AL31" s="26"/>
+      <c r="AC31" s="31"/>
+      <c r="AD31" s="31"/>
+      <c r="AE31" s="31"/>
+      <c r="AF31" s="31"/>
+      <c r="AG31" s="31"/>
+      <c r="AH31" s="31"/>
+      <c r="AI31" s="31"/>
+      <c r="AJ31" s="31"/>
+      <c r="AK31" s="31"/>
+      <c r="AL31" s="32"/>
       <c r="AM31" s="13"/>
       <c r="AO31" s="12"/>
       <c r="AS31" s="20"/>
       <c r="AT31" s="20"/>
       <c r="AU31" s="20"/>
-      <c r="AV31" s="30" t="s">
+      <c r="AV31" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AW31" s="31"/>
-      <c r="AX31" s="31"/>
-      <c r="AY31" s="31"/>
-      <c r="AZ31" s="31"/>
-      <c r="BA31" s="32"/>
+      <c r="AW31" s="25"/>
+      <c r="AX31" s="25"/>
+      <c r="AY31" s="25"/>
+      <c r="AZ31" s="25"/>
+      <c r="BA31" s="26"/>
       <c r="BB31" s="20"/>
-      <c r="BC31" s="30" t="s">
+      <c r="BC31" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="BD31" s="31"/>
-      <c r="BE31" s="31"/>
-      <c r="BF31" s="31"/>
-      <c r="BG31" s="31"/>
-      <c r="BH31" s="32"/>
+      <c r="BD31" s="25"/>
+      <c r="BE31" s="25"/>
+      <c r="BF31" s="25"/>
+      <c r="BG31" s="25"/>
+      <c r="BH31" s="26"/>
       <c r="BI31" s="20"/>
-      <c r="BJ31" s="30" t="s">
+      <c r="BJ31" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="BK31" s="31"/>
-      <c r="BL31" s="31"/>
-      <c r="BM31" s="31"/>
-      <c r="BN31" s="31"/>
-      <c r="BO31" s="32"/>
+      <c r="BK31" s="25"/>
+      <c r="BL31" s="25"/>
+      <c r="BM31" s="25"/>
+      <c r="BN31" s="25"/>
+      <c r="BO31" s="26"/>
       <c r="BP31" s="20"/>
       <c r="BQ31" s="20"/>
       <c r="BR31" s="20"/>
       <c r="BV31" s="13"/>
       <c r="BX31" s="12"/>
-      <c r="BY31" s="30" t="s">
+      <c r="BY31" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="BZ31" s="31"/>
-      <c r="CA31" s="31"/>
-      <c r="CB31" s="31"/>
-      <c r="CC31" s="31"/>
-      <c r="CD31" s="31"/>
-      <c r="CE31" s="31"/>
-      <c r="CF31" s="31"/>
-      <c r="CG31" s="31"/>
-      <c r="CH31" s="31"/>
-      <c r="CI31" s="31"/>
-      <c r="CJ31" s="31"/>
-      <c r="CK31" s="32"/>
+      <c r="BZ31" s="25"/>
+      <c r="CA31" s="25"/>
+      <c r="CB31" s="25"/>
+      <c r="CC31" s="25"/>
+      <c r="CD31" s="25"/>
+      <c r="CE31" s="25"/>
+      <c r="CF31" s="25"/>
+      <c r="CG31" s="25"/>
+      <c r="CH31" s="25"/>
+      <c r="CI31" s="25"/>
+      <c r="CJ31" s="25"/>
+      <c r="CK31" s="26"/>
       <c r="CL31" s="13"/>
       <c r="CM31" s="13"/>
       <c r="CN31" s="2">
@@ -3641,46 +3641,46 @@
       </c>
       <c r="V32" s="12"/>
       <c r="W32" s="12"/>
-      <c r="X32" s="27"/>
-      <c r="Y32" s="28"/>
-      <c r="Z32" s="28"/>
-      <c r="AA32" s="29"/>
-      <c r="AB32" s="27"/>
-      <c r="AC32" s="28"/>
-      <c r="AD32" s="28"/>
-      <c r="AE32" s="28"/>
-      <c r="AF32" s="28"/>
-      <c r="AG32" s="28"/>
-      <c r="AH32" s="28"/>
-      <c r="AI32" s="28"/>
-      <c r="AJ32" s="28"/>
-      <c r="AK32" s="28"/>
-      <c r="AL32" s="29"/>
+      <c r="X32" s="33"/>
+      <c r="Y32" s="34"/>
+      <c r="Z32" s="34"/>
+      <c r="AA32" s="35"/>
+      <c r="AB32" s="33"/>
+      <c r="AC32" s="34"/>
+      <c r="AD32" s="34"/>
+      <c r="AE32" s="34"/>
+      <c r="AF32" s="34"/>
+      <c r="AG32" s="34"/>
+      <c r="AH32" s="34"/>
+      <c r="AI32" s="34"/>
+      <c r="AJ32" s="34"/>
+      <c r="AK32" s="34"/>
+      <c r="AL32" s="35"/>
       <c r="AM32" s="13"/>
       <c r="AO32" s="12"/>
       <c r="AS32" s="20"/>
       <c r="AT32" s="20"/>
       <c r="AU32" s="20"/>
-      <c r="AV32" s="33"/>
-      <c r="AW32" s="34"/>
-      <c r="AX32" s="34"/>
-      <c r="AY32" s="34"/>
-      <c r="AZ32" s="34"/>
-      <c r="BA32" s="35"/>
+      <c r="AV32" s="27"/>
+      <c r="AW32" s="28"/>
+      <c r="AX32" s="28"/>
+      <c r="AY32" s="28"/>
+      <c r="AZ32" s="28"/>
+      <c r="BA32" s="29"/>
       <c r="BB32" s="20"/>
-      <c r="BC32" s="33"/>
-      <c r="BD32" s="34"/>
-      <c r="BE32" s="34"/>
-      <c r="BF32" s="34"/>
-      <c r="BG32" s="34"/>
-      <c r="BH32" s="35"/>
+      <c r="BC32" s="27"/>
+      <c r="BD32" s="28"/>
+      <c r="BE32" s="28"/>
+      <c r="BF32" s="28"/>
+      <c r="BG32" s="28"/>
+      <c r="BH32" s="29"/>
       <c r="BI32" s="20"/>
-      <c r="BJ32" s="33"/>
-      <c r="BK32" s="34"/>
-      <c r="BL32" s="34"/>
-      <c r="BM32" s="34"/>
-      <c r="BN32" s="34"/>
-      <c r="BO32" s="35"/>
+      <c r="BJ32" s="27"/>
+      <c r="BK32" s="28"/>
+      <c r="BL32" s="28"/>
+      <c r="BM32" s="28"/>
+      <c r="BN32" s="28"/>
+      <c r="BO32" s="29"/>
       <c r="BP32" s="20"/>
       <c r="BQ32" s="20"/>
       <c r="BR32" s="20"/>
@@ -3737,19 +3737,19 @@
       <c r="AO33" s="12"/>
       <c r="BV33" s="13"/>
       <c r="BX33" s="12"/>
-      <c r="BY33" s="33"/>
-      <c r="BZ33" s="34"/>
-      <c r="CA33" s="34"/>
-      <c r="CB33" s="34"/>
-      <c r="CC33" s="34"/>
-      <c r="CD33" s="34"/>
-      <c r="CE33" s="34"/>
-      <c r="CF33" s="34"/>
-      <c r="CG33" s="34"/>
-      <c r="CH33" s="34"/>
-      <c r="CI33" s="34"/>
-      <c r="CJ33" s="34"/>
-      <c r="CK33" s="35"/>
+      <c r="BY33" s="27"/>
+      <c r="BZ33" s="28"/>
+      <c r="CA33" s="28"/>
+      <c r="CB33" s="28"/>
+      <c r="CC33" s="28"/>
+      <c r="CD33" s="28"/>
+      <c r="CE33" s="28"/>
+      <c r="CF33" s="28"/>
+      <c r="CG33" s="28"/>
+      <c r="CH33" s="28"/>
+      <c r="CI33" s="28"/>
+      <c r="CJ33" s="28"/>
+      <c r="CK33" s="29"/>
       <c r="CL33" s="13"/>
       <c r="CM33" s="13"/>
       <c r="CN33" s="2">
@@ -3913,63 +3913,63 @@
         <v>29</v>
       </c>
       <c r="V36" s="12"/>
-      <c r="W36" s="24" t="s">
+      <c r="W36" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="X36" s="25"/>
-      <c r="Y36" s="25"/>
-      <c r="Z36" s="25"/>
-      <c r="AA36" s="25"/>
-      <c r="AB36" s="25"/>
-      <c r="AC36" s="25"/>
-      <c r="AD36" s="25"/>
-      <c r="AE36" s="25"/>
-      <c r="AF36" s="26"/>
+      <c r="X36" s="31"/>
+      <c r="Y36" s="31"/>
+      <c r="Z36" s="31"/>
+      <c r="AA36" s="31"/>
+      <c r="AB36" s="31"/>
+      <c r="AC36" s="31"/>
+      <c r="AD36" s="31"/>
+      <c r="AE36" s="31"/>
+      <c r="AF36" s="32"/>
       <c r="AG36" s="20"/>
-      <c r="AH36" s="24" t="s">
+      <c r="AH36" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="AI36" s="25"/>
-      <c r="AJ36" s="26"/>
-      <c r="AK36" s="30" t="s">
+      <c r="AI36" s="31"/>
+      <c r="AJ36" s="32"/>
+      <c r="AK36" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="AL36" s="31"/>
-      <c r="AM36" s="31"/>
-      <c r="AN36" s="32"/>
+      <c r="AL36" s="25"/>
+      <c r="AM36" s="25"/>
+      <c r="AN36" s="26"/>
       <c r="AO36" s="20"/>
-      <c r="AP36" s="30" t="s">
+      <c r="AP36" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="AQ36" s="32"/>
+      <c r="AQ36" s="26"/>
       <c r="AS36" s="20"/>
-      <c r="AT36" s="24" t="s">
+      <c r="AT36" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="AU36" s="25"/>
-      <c r="AV36" s="26"/>
-      <c r="AW36" s="31" t="s">
+      <c r="AU36" s="31"/>
+      <c r="AV36" s="32"/>
+      <c r="AW36" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="AX36" s="31"/>
-      <c r="AY36" s="31"/>
-      <c r="AZ36" s="31"/>
-      <c r="BA36" s="31"/>
-      <c r="BB36" s="31"/>
-      <c r="BC36" s="31"/>
-      <c r="BD36" s="32"/>
-      <c r="BF36" s="24" t="s">
+      <c r="AX36" s="25"/>
+      <c r="AY36" s="25"/>
+      <c r="AZ36" s="25"/>
+      <c r="BA36" s="25"/>
+      <c r="BB36" s="25"/>
+      <c r="BC36" s="25"/>
+      <c r="BD36" s="26"/>
+      <c r="BF36" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="BG36" s="25"/>
-      <c r="BH36" s="25"/>
-      <c r="BI36" s="25"/>
-      <c r="BJ36" s="25"/>
-      <c r="BK36" s="25"/>
-      <c r="BL36" s="25"/>
-      <c r="BM36" s="25"/>
-      <c r="BN36" s="25"/>
-      <c r="BO36" s="26"/>
+      <c r="BG36" s="31"/>
+      <c r="BH36" s="31"/>
+      <c r="BI36" s="31"/>
+      <c r="BJ36" s="31"/>
+      <c r="BK36" s="31"/>
+      <c r="BL36" s="31"/>
+      <c r="BM36" s="31"/>
+      <c r="BN36" s="31"/>
+      <c r="BO36" s="32"/>
       <c r="BP36" s="20"/>
       <c r="BQ36" s="20"/>
       <c r="BR36" s="20"/>
@@ -4025,49 +4025,49 @@
         <v>30</v>
       </c>
       <c r="V37" s="12"/>
-      <c r="W37" s="27"/>
-      <c r="X37" s="28"/>
-      <c r="Y37" s="28"/>
-      <c r="Z37" s="28"/>
-      <c r="AA37" s="28"/>
-      <c r="AB37" s="28"/>
-      <c r="AC37" s="28"/>
-      <c r="AD37" s="28"/>
-      <c r="AE37" s="28"/>
-      <c r="AF37" s="29"/>
+      <c r="W37" s="33"/>
+      <c r="X37" s="34"/>
+      <c r="Y37" s="34"/>
+      <c r="Z37" s="34"/>
+      <c r="AA37" s="34"/>
+      <c r="AB37" s="34"/>
+      <c r="AC37" s="34"/>
+      <c r="AD37" s="34"/>
+      <c r="AE37" s="34"/>
+      <c r="AF37" s="35"/>
       <c r="AG37" s="20"/>
-      <c r="AH37" s="27"/>
-      <c r="AI37" s="28"/>
-      <c r="AJ37" s="29"/>
-      <c r="AK37" s="33"/>
-      <c r="AL37" s="34"/>
-      <c r="AM37" s="34"/>
-      <c r="AN37" s="35"/>
+      <c r="AH37" s="33"/>
+      <c r="AI37" s="34"/>
+      <c r="AJ37" s="35"/>
+      <c r="AK37" s="27"/>
+      <c r="AL37" s="28"/>
+      <c r="AM37" s="28"/>
+      <c r="AN37" s="29"/>
       <c r="AO37" s="20"/>
-      <c r="AP37" s="33"/>
-      <c r="AQ37" s="35"/>
+      <c r="AP37" s="27"/>
+      <c r="AQ37" s="29"/>
       <c r="AS37" s="20"/>
-      <c r="AT37" s="27"/>
-      <c r="AU37" s="28"/>
-      <c r="AV37" s="29"/>
-      <c r="AW37" s="34"/>
-      <c r="AX37" s="34"/>
-      <c r="AY37" s="34"/>
-      <c r="AZ37" s="34"/>
-      <c r="BA37" s="34"/>
-      <c r="BB37" s="34"/>
-      <c r="BC37" s="34"/>
-      <c r="BD37" s="35"/>
-      <c r="BF37" s="27"/>
-      <c r="BG37" s="28"/>
-      <c r="BH37" s="28"/>
-      <c r="BI37" s="28"/>
-      <c r="BJ37" s="28"/>
-      <c r="BK37" s="28"/>
-      <c r="BL37" s="28"/>
-      <c r="BM37" s="28"/>
-      <c r="BN37" s="28"/>
-      <c r="BO37" s="29"/>
+      <c r="AT37" s="33"/>
+      <c r="AU37" s="34"/>
+      <c r="AV37" s="35"/>
+      <c r="AW37" s="28"/>
+      <c r="AX37" s="28"/>
+      <c r="AY37" s="28"/>
+      <c r="AZ37" s="28"/>
+      <c r="BA37" s="28"/>
+      <c r="BB37" s="28"/>
+      <c r="BC37" s="28"/>
+      <c r="BD37" s="29"/>
+      <c r="BF37" s="33"/>
+      <c r="BG37" s="34"/>
+      <c r="BH37" s="34"/>
+      <c r="BI37" s="34"/>
+      <c r="BJ37" s="34"/>
+      <c r="BK37" s="34"/>
+      <c r="BL37" s="34"/>
+      <c r="BM37" s="34"/>
+      <c r="BN37" s="34"/>
+      <c r="BO37" s="35"/>
       <c r="BP37" s="20"/>
       <c r="BQ37" s="20"/>
       <c r="BR37" s="20"/>
@@ -4257,42 +4257,42 @@
       <c r="W40" s="12"/>
       <c r="BD40" s="13"/>
       <c r="BF40" s="12"/>
-      <c r="BG40" s="24" t="s">
+      <c r="BG40" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="BH40" s="25"/>
-      <c r="BI40" s="25"/>
-      <c r="BJ40" s="25"/>
-      <c r="BK40" s="25"/>
-      <c r="BL40" s="25"/>
-      <c r="BM40" s="25"/>
-      <c r="BN40" s="25"/>
-      <c r="BO40" s="25"/>
-      <c r="BP40" s="25"/>
-      <c r="BQ40" s="25"/>
-      <c r="BR40" s="25"/>
-      <c r="BS40" s="25"/>
-      <c r="BT40" s="25"/>
-      <c r="BU40" s="25"/>
-      <c r="BV40" s="25"/>
-      <c r="BW40" s="25"/>
-      <c r="BX40" s="25"/>
-      <c r="BY40" s="26"/>
+      <c r="BH40" s="31"/>
+      <c r="BI40" s="31"/>
+      <c r="BJ40" s="31"/>
+      <c r="BK40" s="31"/>
+      <c r="BL40" s="31"/>
+      <c r="BM40" s="31"/>
+      <c r="BN40" s="31"/>
+      <c r="BO40" s="31"/>
+      <c r="BP40" s="31"/>
+      <c r="BQ40" s="31"/>
+      <c r="BR40" s="31"/>
+      <c r="BS40" s="31"/>
+      <c r="BT40" s="31"/>
+      <c r="BU40" s="31"/>
+      <c r="BV40" s="31"/>
+      <c r="BW40" s="31"/>
+      <c r="BX40" s="31"/>
+      <c r="BY40" s="32"/>
       <c r="BZ40" s="20"/>
-      <c r="CA40" s="30" t="s">
+      <c r="CA40" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="CB40" s="31"/>
-      <c r="CC40" s="31"/>
-      <c r="CD40" s="31"/>
-      <c r="CE40" s="32"/>
-      <c r="CG40" s="30" t="s">
+      <c r="CB40" s="25"/>
+      <c r="CC40" s="25"/>
+      <c r="CD40" s="25"/>
+      <c r="CE40" s="26"/>
+      <c r="CG40" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="CH40" s="31"/>
-      <c r="CI40" s="31"/>
-      <c r="CJ40" s="31"/>
-      <c r="CK40" s="32"/>
+      <c r="CH40" s="25"/>
+      <c r="CI40" s="25"/>
+      <c r="CJ40" s="25"/>
+      <c r="CK40" s="26"/>
       <c r="CL40" s="13"/>
       <c r="CM40" s="13"/>
       <c r="CN40" s="2">
@@ -4329,36 +4329,36 @@
       <c r="W41" s="12"/>
       <c r="BD41" s="13"/>
       <c r="BF41" s="12"/>
-      <c r="BG41" s="27"/>
-      <c r="BH41" s="28"/>
-      <c r="BI41" s="28"/>
-      <c r="BJ41" s="28"/>
-      <c r="BK41" s="28"/>
-      <c r="BL41" s="28"/>
-      <c r="BM41" s="28"/>
-      <c r="BN41" s="28"/>
-      <c r="BO41" s="28"/>
-      <c r="BP41" s="28"/>
-      <c r="BQ41" s="28"/>
-      <c r="BR41" s="28"/>
-      <c r="BS41" s="28"/>
-      <c r="BT41" s="28"/>
-      <c r="BU41" s="28"/>
-      <c r="BV41" s="28"/>
-      <c r="BW41" s="28"/>
-      <c r="BX41" s="28"/>
-      <c r="BY41" s="29"/>
+      <c r="BG41" s="33"/>
+      <c r="BH41" s="34"/>
+      <c r="BI41" s="34"/>
+      <c r="BJ41" s="34"/>
+      <c r="BK41" s="34"/>
+      <c r="BL41" s="34"/>
+      <c r="BM41" s="34"/>
+      <c r="BN41" s="34"/>
+      <c r="BO41" s="34"/>
+      <c r="BP41" s="34"/>
+      <c r="BQ41" s="34"/>
+      <c r="BR41" s="34"/>
+      <c r="BS41" s="34"/>
+      <c r="BT41" s="34"/>
+      <c r="BU41" s="34"/>
+      <c r="BV41" s="34"/>
+      <c r="BW41" s="34"/>
+      <c r="BX41" s="34"/>
+      <c r="BY41" s="35"/>
       <c r="BZ41" s="20"/>
-      <c r="CA41" s="33"/>
-      <c r="CB41" s="34"/>
-      <c r="CC41" s="34"/>
-      <c r="CD41" s="34"/>
-      <c r="CE41" s="35"/>
-      <c r="CG41" s="33"/>
-      <c r="CH41" s="34"/>
-      <c r="CI41" s="34"/>
-      <c r="CJ41" s="34"/>
-      <c r="CK41" s="35"/>
+      <c r="CA41" s="27"/>
+      <c r="CB41" s="28"/>
+      <c r="CC41" s="28"/>
+      <c r="CD41" s="28"/>
+      <c r="CE41" s="29"/>
+      <c r="CG41" s="27"/>
+      <c r="CH41" s="28"/>
+      <c r="CI41" s="28"/>
+      <c r="CJ41" s="28"/>
+      <c r="CK41" s="29"/>
       <c r="CL41" s="13"/>
       <c r="CM41" s="13"/>
       <c r="CN41" s="2">
@@ -4431,42 +4431,42 @@
       <c r="W43" s="12"/>
       <c r="BD43" s="13"/>
       <c r="BF43" s="12"/>
-      <c r="BG43" s="30" t="s">
+      <c r="BG43" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="BH43" s="31"/>
-      <c r="BI43" s="31"/>
-      <c r="BJ43" s="31"/>
-      <c r="BK43" s="31"/>
-      <c r="BL43" s="31"/>
-      <c r="BM43" s="31"/>
-      <c r="BN43" s="31"/>
-      <c r="BO43" s="31"/>
-      <c r="BP43" s="31"/>
-      <c r="BQ43" s="31"/>
-      <c r="BR43" s="31"/>
-      <c r="BS43" s="31"/>
-      <c r="BT43" s="31"/>
-      <c r="BU43" s="31"/>
-      <c r="BV43" s="31"/>
-      <c r="BW43" s="31"/>
-      <c r="BX43" s="31"/>
-      <c r="BY43" s="32"/>
+      <c r="BH43" s="25"/>
+      <c r="BI43" s="25"/>
+      <c r="BJ43" s="25"/>
+      <c r="BK43" s="25"/>
+      <c r="BL43" s="25"/>
+      <c r="BM43" s="25"/>
+      <c r="BN43" s="25"/>
+      <c r="BO43" s="25"/>
+      <c r="BP43" s="25"/>
+      <c r="BQ43" s="25"/>
+      <c r="BR43" s="25"/>
+      <c r="BS43" s="25"/>
+      <c r="BT43" s="25"/>
+      <c r="BU43" s="25"/>
+      <c r="BV43" s="25"/>
+      <c r="BW43" s="25"/>
+      <c r="BX43" s="25"/>
+      <c r="BY43" s="26"/>
       <c r="BZ43" s="20"/>
-      <c r="CA43" s="30" t="s">
+      <c r="CA43" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="CB43" s="31"/>
-      <c r="CC43" s="31"/>
-      <c r="CD43" s="31"/>
-      <c r="CE43" s="32"/>
-      <c r="CG43" s="30" t="s">
+      <c r="CB43" s="25"/>
+      <c r="CC43" s="25"/>
+      <c r="CD43" s="25"/>
+      <c r="CE43" s="26"/>
+      <c r="CG43" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="CH43" s="31"/>
-      <c r="CI43" s="31"/>
-      <c r="CJ43" s="31"/>
-      <c r="CK43" s="32"/>
+      <c r="CH43" s="25"/>
+      <c r="CI43" s="25"/>
+      <c r="CJ43" s="25"/>
+      <c r="CK43" s="26"/>
       <c r="CL43" s="13"/>
       <c r="CM43" s="13"/>
       <c r="CN43" s="2">
@@ -4503,36 +4503,36 @@
       <c r="W44" s="12"/>
       <c r="BD44" s="13"/>
       <c r="BF44" s="12"/>
-      <c r="BG44" s="33"/>
-      <c r="BH44" s="34"/>
-      <c r="BI44" s="34"/>
-      <c r="BJ44" s="34"/>
-      <c r="BK44" s="34"/>
-      <c r="BL44" s="34"/>
-      <c r="BM44" s="34"/>
-      <c r="BN44" s="34"/>
-      <c r="BO44" s="34"/>
-      <c r="BP44" s="34"/>
-      <c r="BQ44" s="34"/>
-      <c r="BR44" s="34"/>
-      <c r="BS44" s="34"/>
-      <c r="BT44" s="34"/>
-      <c r="BU44" s="34"/>
-      <c r="BV44" s="34"/>
-      <c r="BW44" s="34"/>
-      <c r="BX44" s="34"/>
-      <c r="BY44" s="35"/>
+      <c r="BG44" s="27"/>
+      <c r="BH44" s="28"/>
+      <c r="BI44" s="28"/>
+      <c r="BJ44" s="28"/>
+      <c r="BK44" s="28"/>
+      <c r="BL44" s="28"/>
+      <c r="BM44" s="28"/>
+      <c r="BN44" s="28"/>
+      <c r="BO44" s="28"/>
+      <c r="BP44" s="28"/>
+      <c r="BQ44" s="28"/>
+      <c r="BR44" s="28"/>
+      <c r="BS44" s="28"/>
+      <c r="BT44" s="28"/>
+      <c r="BU44" s="28"/>
+      <c r="BV44" s="28"/>
+      <c r="BW44" s="28"/>
+      <c r="BX44" s="28"/>
+      <c r="BY44" s="29"/>
       <c r="BZ44" s="20"/>
-      <c r="CA44" s="33"/>
-      <c r="CB44" s="34"/>
-      <c r="CC44" s="34"/>
-      <c r="CD44" s="34"/>
-      <c r="CE44" s="35"/>
-      <c r="CG44" s="33"/>
-      <c r="CH44" s="34"/>
-      <c r="CI44" s="34"/>
-      <c r="CJ44" s="34"/>
-      <c r="CK44" s="35"/>
+      <c r="CA44" s="27"/>
+      <c r="CB44" s="28"/>
+      <c r="CC44" s="28"/>
+      <c r="CD44" s="28"/>
+      <c r="CE44" s="29"/>
+      <c r="CG44" s="27"/>
+      <c r="CH44" s="28"/>
+      <c r="CI44" s="28"/>
+      <c r="CJ44" s="28"/>
+      <c r="CK44" s="29"/>
       <c r="CL44" s="13"/>
       <c r="CM44" s="13"/>
       <c r="CN44" s="2">
@@ -4605,25 +4605,25 @@
       <c r="W46" s="12"/>
       <c r="BD46" s="13"/>
       <c r="BF46" s="12"/>
-      <c r="BG46" s="24" t="s">
+      <c r="BG46" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="BH46" s="25"/>
-      <c r="BI46" s="25"/>
-      <c r="BJ46" s="25"/>
-      <c r="BK46" s="25"/>
-      <c r="BL46" s="25"/>
-      <c r="BM46" s="25"/>
-      <c r="BN46" s="25"/>
-      <c r="BO46" s="25"/>
-      <c r="BP46" s="26"/>
-      <c r="CA46" s="30" t="s">
+      <c r="BH46" s="31"/>
+      <c r="BI46" s="31"/>
+      <c r="BJ46" s="31"/>
+      <c r="BK46" s="31"/>
+      <c r="BL46" s="31"/>
+      <c r="BM46" s="31"/>
+      <c r="BN46" s="31"/>
+      <c r="BO46" s="31"/>
+      <c r="BP46" s="32"/>
+      <c r="CA46" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="CB46" s="31"/>
-      <c r="CC46" s="31"/>
-      <c r="CD46" s="31"/>
-      <c r="CE46" s="32"/>
+      <c r="CB46" s="25"/>
+      <c r="CC46" s="25"/>
+      <c r="CD46" s="25"/>
+      <c r="CE46" s="26"/>
       <c r="CG46" s="20"/>
       <c r="CH46" s="20"/>
       <c r="CI46" s="20"/>
@@ -4665,21 +4665,21 @@
       <c r="W47" s="12"/>
       <c r="BD47" s="13"/>
       <c r="BF47" s="12"/>
-      <c r="BG47" s="27"/>
-      <c r="BH47" s="28"/>
-      <c r="BI47" s="28"/>
-      <c r="BJ47" s="28"/>
-      <c r="BK47" s="28"/>
-      <c r="BL47" s="28"/>
-      <c r="BM47" s="28"/>
-      <c r="BN47" s="28"/>
-      <c r="BO47" s="28"/>
-      <c r="BP47" s="29"/>
-      <c r="CA47" s="33"/>
-      <c r="CB47" s="34"/>
-      <c r="CC47" s="34"/>
-      <c r="CD47" s="34"/>
-      <c r="CE47" s="35"/>
+      <c r="BG47" s="33"/>
+      <c r="BH47" s="34"/>
+      <c r="BI47" s="34"/>
+      <c r="BJ47" s="34"/>
+      <c r="BK47" s="34"/>
+      <c r="BL47" s="34"/>
+      <c r="BM47" s="34"/>
+      <c r="BN47" s="34"/>
+      <c r="BO47" s="34"/>
+      <c r="BP47" s="35"/>
+      <c r="CA47" s="27"/>
+      <c r="CB47" s="28"/>
+      <c r="CC47" s="28"/>
+      <c r="CD47" s="28"/>
+      <c r="CE47" s="29"/>
       <c r="CG47" s="20"/>
       <c r="CH47" s="20"/>
       <c r="CI47" s="20"/>
@@ -4854,18 +4854,18 @@
       <c r="V50" s="12"/>
       <c r="W50" s="12"/>
       <c r="BD50" s="13"/>
-      <c r="BF50" s="24" t="s">
+      <c r="BF50" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="BG50" s="25"/>
-      <c r="BH50" s="25"/>
-      <c r="BI50" s="25"/>
-      <c r="BJ50" s="25"/>
-      <c r="BK50" s="25"/>
-      <c r="BL50" s="25"/>
-      <c r="BM50" s="25"/>
-      <c r="BN50" s="25"/>
-      <c r="BO50" s="26"/>
+      <c r="BG50" s="31"/>
+      <c r="BH50" s="31"/>
+      <c r="BI50" s="31"/>
+      <c r="BJ50" s="31"/>
+      <c r="BK50" s="31"/>
+      <c r="BL50" s="31"/>
+      <c r="BM50" s="31"/>
+      <c r="BN50" s="31"/>
+      <c r="BO50" s="32"/>
       <c r="BP50" s="20"/>
       <c r="BQ50" s="20"/>
       <c r="BR50" s="20"/>
@@ -4874,22 +4874,22 @@
       <c r="BU50" s="20"/>
       <c r="BY50" s="20"/>
       <c r="BZ50" s="20"/>
-      <c r="CA50" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="CB50" s="31"/>
-      <c r="CC50" s="31"/>
-      <c r="CD50" s="31"/>
-      <c r="CE50" s="31"/>
-      <c r="CF50" s="31"/>
-      <c r="CG50" s="32"/>
-      <c r="CH50" s="30" t="s">
+      <c r="CA50" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="CB50" s="25"/>
+      <c r="CC50" s="25"/>
+      <c r="CD50" s="25"/>
+      <c r="CE50" s="25"/>
+      <c r="CF50" s="25"/>
+      <c r="CG50" s="26"/>
+      <c r="CH50" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="CI50" s="31"/>
-      <c r="CJ50" s="31"/>
-      <c r="CK50" s="31"/>
-      <c r="CL50" s="32"/>
+      <c r="CI50" s="25"/>
+      <c r="CJ50" s="25"/>
+      <c r="CK50" s="25"/>
+      <c r="CL50" s="26"/>
       <c r="CM50" s="13"/>
       <c r="CN50" s="2">
         <f t="shared" si="7"/>
@@ -4924,16 +4924,16 @@
       <c r="V51" s="12"/>
       <c r="W51" s="12"/>
       <c r="BD51" s="13"/>
-      <c r="BF51" s="27"/>
-      <c r="BG51" s="28"/>
-      <c r="BH51" s="28"/>
-      <c r="BI51" s="28"/>
-      <c r="BJ51" s="28"/>
-      <c r="BK51" s="28"/>
-      <c r="BL51" s="28"/>
-      <c r="BM51" s="28"/>
-      <c r="BN51" s="28"/>
-      <c r="BO51" s="29"/>
+      <c r="BF51" s="33"/>
+      <c r="BG51" s="34"/>
+      <c r="BH51" s="34"/>
+      <c r="BI51" s="34"/>
+      <c r="BJ51" s="34"/>
+      <c r="BK51" s="34"/>
+      <c r="BL51" s="34"/>
+      <c r="BM51" s="34"/>
+      <c r="BN51" s="34"/>
+      <c r="BO51" s="35"/>
       <c r="BP51" s="20"/>
       <c r="BQ51" s="20"/>
       <c r="BR51" s="20"/>
@@ -4942,18 +4942,18 @@
       <c r="BU51" s="20"/>
       <c r="BY51" s="20"/>
       <c r="BZ51" s="20"/>
-      <c r="CA51" s="33"/>
-      <c r="CB51" s="34"/>
-      <c r="CC51" s="34"/>
-      <c r="CD51" s="34"/>
-      <c r="CE51" s="34"/>
-      <c r="CF51" s="34"/>
-      <c r="CG51" s="35"/>
-      <c r="CH51" s="33"/>
-      <c r="CI51" s="34"/>
-      <c r="CJ51" s="34"/>
-      <c r="CK51" s="34"/>
-      <c r="CL51" s="35"/>
+      <c r="CA51" s="27"/>
+      <c r="CB51" s="28"/>
+      <c r="CC51" s="28"/>
+      <c r="CD51" s="28"/>
+      <c r="CE51" s="28"/>
+      <c r="CF51" s="28"/>
+      <c r="CG51" s="29"/>
+      <c r="CH51" s="27"/>
+      <c r="CI51" s="28"/>
+      <c r="CJ51" s="28"/>
+      <c r="CK51" s="28"/>
+      <c r="CL51" s="29"/>
       <c r="CM51" s="13"/>
       <c r="CN51" s="2">
         <f t="shared" si="7"/>
@@ -5091,13 +5091,13 @@
       <c r="BD54" s="13"/>
       <c r="BF54" s="12"/>
       <c r="CE54" s="11"/>
-      <c r="CG54" s="30" t="s">
+      <c r="CG54" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="CH54" s="31"/>
-      <c r="CI54" s="31"/>
-      <c r="CJ54" s="31"/>
-      <c r="CK54" s="32"/>
+      <c r="CH54" s="25"/>
+      <c r="CI54" s="25"/>
+      <c r="CJ54" s="25"/>
+      <c r="CK54" s="26"/>
       <c r="CL54" s="13"/>
       <c r="CM54" s="13"/>
       <c r="CN54" s="2">
@@ -5135,11 +5135,11 @@
       <c r="BD55" s="13"/>
       <c r="BF55" s="12"/>
       <c r="CE55" s="11"/>
-      <c r="CG55" s="33"/>
-      <c r="CH55" s="34"/>
-      <c r="CI55" s="34"/>
-      <c r="CJ55" s="34"/>
-      <c r="CK55" s="35"/>
+      <c r="CG55" s="27"/>
+      <c r="CH55" s="28"/>
+      <c r="CI55" s="28"/>
+      <c r="CJ55" s="28"/>
+      <c r="CK55" s="29"/>
       <c r="CL55" s="13"/>
       <c r="CM55" s="13"/>
       <c r="CN55" s="2">
@@ -5214,13 +5214,13 @@
       <c r="BD57" s="13"/>
       <c r="BF57" s="12"/>
       <c r="CE57" s="11"/>
-      <c r="CG57" s="30" t="s">
+      <c r="CG57" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="CH57" s="31"/>
-      <c r="CI57" s="31"/>
-      <c r="CJ57" s="31"/>
-      <c r="CK57" s="32"/>
+      <c r="CH57" s="25"/>
+      <c r="CI57" s="25"/>
+      <c r="CJ57" s="25"/>
+      <c r="CK57" s="26"/>
       <c r="CL57" s="13"/>
       <c r="CM57" s="13"/>
       <c r="CN57" s="2">
@@ -5258,11 +5258,11 @@
       <c r="BD58" s="13"/>
       <c r="BF58" s="12"/>
       <c r="CE58" s="11"/>
-      <c r="CG58" s="33"/>
-      <c r="CH58" s="34"/>
-      <c r="CI58" s="34"/>
-      <c r="CJ58" s="34"/>
-      <c r="CK58" s="35"/>
+      <c r="CG58" s="27"/>
+      <c r="CH58" s="28"/>
+      <c r="CI58" s="28"/>
+      <c r="CJ58" s="28"/>
+      <c r="CK58" s="29"/>
       <c r="CL58" s="13"/>
       <c r="CM58" s="13"/>
       <c r="CN58" s="2">
@@ -5337,13 +5337,13 @@
       <c r="BD60" s="13"/>
       <c r="BF60" s="12"/>
       <c r="CE60" s="11"/>
-      <c r="CG60" s="30" t="s">
+      <c r="CG60" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="CH60" s="31"/>
-      <c r="CI60" s="31"/>
-      <c r="CJ60" s="31"/>
-      <c r="CK60" s="32"/>
+      <c r="CH60" s="25"/>
+      <c r="CI60" s="25"/>
+      <c r="CJ60" s="25"/>
+      <c r="CK60" s="26"/>
       <c r="CL60" s="13"/>
       <c r="CM60" s="13"/>
       <c r="CN60" s="2">
@@ -5381,11 +5381,11 @@
       <c r="BD61" s="13"/>
       <c r="BF61" s="12"/>
       <c r="CE61" s="11"/>
-      <c r="CG61" s="33"/>
-      <c r="CH61" s="34"/>
-      <c r="CI61" s="34"/>
-      <c r="CJ61" s="34"/>
-      <c r="CK61" s="35"/>
+      <c r="CG61" s="27"/>
+      <c r="CH61" s="28"/>
+      <c r="CI61" s="28"/>
+      <c r="CJ61" s="28"/>
+      <c r="CK61" s="29"/>
       <c r="CL61" s="13"/>
       <c r="CM61" s="13"/>
       <c r="CN61" s="2">
@@ -5460,13 +5460,13 @@
       <c r="BD63" s="13"/>
       <c r="BF63" s="12"/>
       <c r="CE63" s="11"/>
-      <c r="CG63" s="30" t="s">
+      <c r="CG63" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="CH63" s="31"/>
-      <c r="CI63" s="31"/>
-      <c r="CJ63" s="31"/>
-      <c r="CK63" s="32"/>
+      <c r="CH63" s="25"/>
+      <c r="CI63" s="25"/>
+      <c r="CJ63" s="25"/>
+      <c r="CK63" s="26"/>
       <c r="CL63" s="13"/>
       <c r="CM63" s="13"/>
       <c r="CN63" s="2">
@@ -5504,11 +5504,11 @@
       <c r="BD64" s="13"/>
       <c r="BF64" s="12"/>
       <c r="CE64" s="11"/>
-      <c r="CG64" s="33"/>
-      <c r="CH64" s="34"/>
-      <c r="CI64" s="34"/>
-      <c r="CJ64" s="34"/>
-      <c r="CK64" s="35"/>
+      <c r="CG64" s="27"/>
+      <c r="CH64" s="28"/>
+      <c r="CI64" s="28"/>
+      <c r="CJ64" s="28"/>
+      <c r="CK64" s="29"/>
       <c r="CL64" s="13"/>
       <c r="CM64" s="13"/>
       <c r="CN64" s="2">
@@ -5583,13 +5583,13 @@
       <c r="BD66" s="13"/>
       <c r="BF66" s="12"/>
       <c r="CE66" s="11"/>
-      <c r="CG66" s="30" t="s">
+      <c r="CG66" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="CH66" s="31"/>
-      <c r="CI66" s="31"/>
-      <c r="CJ66" s="31"/>
-      <c r="CK66" s="32"/>
+      <c r="CH66" s="25"/>
+      <c r="CI66" s="25"/>
+      <c r="CJ66" s="25"/>
+      <c r="CK66" s="26"/>
       <c r="CL66" s="13"/>
       <c r="CM66" s="13"/>
       <c r="CN66" s="2">
@@ -5627,11 +5627,11 @@
       <c r="BD67" s="13"/>
       <c r="BF67" s="12"/>
       <c r="CE67" s="11"/>
-      <c r="CG67" s="33"/>
-      <c r="CH67" s="34"/>
-      <c r="CI67" s="34"/>
-      <c r="CJ67" s="34"/>
-      <c r="CK67" s="35"/>
+      <c r="CG67" s="27"/>
+      <c r="CH67" s="28"/>
+      <c r="CI67" s="28"/>
+      <c r="CJ67" s="28"/>
+      <c r="CK67" s="29"/>
       <c r="CL67" s="13"/>
       <c r="CM67" s="13"/>
       <c r="CN67" s="2">
@@ -6536,14 +6536,14 @@
         <v>83</v>
       </c>
       <c r="V90" s="12"/>
-      <c r="W90" s="30" t="s">
+      <c r="W90" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="X90" s="31"/>
-      <c r="Y90" s="31"/>
-      <c r="Z90" s="31"/>
-      <c r="AA90" s="31"/>
-      <c r="AB90" s="32"/>
+      <c r="X90" s="25"/>
+      <c r="Y90" s="25"/>
+      <c r="Z90" s="25"/>
+      <c r="AA90" s="25"/>
+      <c r="AB90" s="26"/>
       <c r="CM90" s="13"/>
       <c r="CN90" s="2">
         <f t="shared" si="11"/>
@@ -6576,36 +6576,34 @@
         <v>84</v>
       </c>
       <c r="V91" s="12"/>
-      <c r="W91" s="33"/>
-      <c r="X91" s="34"/>
-      <c r="Y91" s="34"/>
-      <c r="Z91" s="34"/>
-      <c r="AA91" s="34"/>
-      <c r="AB91" s="35"/>
-      <c r="AZ91" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="BA91" s="31"/>
-      <c r="BB91" s="31"/>
-      <c r="BC91" s="31"/>
-      <c r="BD91" s="31"/>
-      <c r="BE91" s="31"/>
-      <c r="BF91" s="31"/>
-      <c r="BG91" s="31"/>
-      <c r="BH91" s="31"/>
-      <c r="BI91" s="32"/>
-      <c r="CC91" s="30" t="s">
+      <c r="W91" s="27"/>
+      <c r="X91" s="28"/>
+      <c r="Y91" s="28"/>
+      <c r="Z91" s="28"/>
+      <c r="AA91" s="28"/>
+      <c r="AB91" s="29"/>
+      <c r="AZ91" s="39"/>
+      <c r="BA91" s="39"/>
+      <c r="BB91" s="39"/>
+      <c r="BC91" s="39"/>
+      <c r="BD91" s="39"/>
+      <c r="BE91" s="39"/>
+      <c r="BF91" s="39"/>
+      <c r="BG91" s="39"/>
+      <c r="BH91" s="39"/>
+      <c r="BI91" s="39"/>
+      <c r="CC91" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="CD91" s="31"/>
-      <c r="CE91" s="31"/>
-      <c r="CF91" s="31"/>
-      <c r="CG91" s="31"/>
-      <c r="CH91" s="31"/>
-      <c r="CI91" s="31"/>
-      <c r="CJ91" s="31"/>
-      <c r="CK91" s="31"/>
-      <c r="CL91" s="32"/>
+      <c r="CD91" s="25"/>
+      <c r="CE91" s="25"/>
+      <c r="CF91" s="25"/>
+      <c r="CG91" s="25"/>
+      <c r="CH91" s="25"/>
+      <c r="CI91" s="25"/>
+      <c r="CJ91" s="25"/>
+      <c r="CK91" s="25"/>
+      <c r="CL91" s="26"/>
       <c r="CM91" s="13"/>
       <c r="CN91" s="2">
         <f t="shared" si="11"/>
@@ -6638,16 +6636,16 @@
         <v>85</v>
       </c>
       <c r="V92" s="12"/>
-      <c r="AZ92" s="36"/>
-      <c r="BA92" s="37"/>
-      <c r="BB92" s="37"/>
-      <c r="BC92" s="37"/>
-      <c r="BD92" s="37"/>
-      <c r="BE92" s="37"/>
-      <c r="BF92" s="37"/>
-      <c r="BG92" s="37"/>
-      <c r="BH92" s="37"/>
-      <c r="BI92" s="38"/>
+      <c r="AZ92" s="39"/>
+      <c r="BA92" s="39"/>
+      <c r="BB92" s="39"/>
+      <c r="BC92" s="39"/>
+      <c r="BD92" s="39"/>
+      <c r="BE92" s="39"/>
+      <c r="BF92" s="39"/>
+      <c r="BG92" s="39"/>
+      <c r="BH92" s="39"/>
+      <c r="BI92" s="39"/>
       <c r="CC92" s="36"/>
       <c r="CD92" s="37"/>
       <c r="CE92" s="37"/>
@@ -6690,16 +6688,16 @@
         <v>86</v>
       </c>
       <c r="V93" s="12"/>
-      <c r="AZ93" s="36"/>
-      <c r="BA93" s="37"/>
-      <c r="BB93" s="37"/>
-      <c r="BC93" s="37"/>
-      <c r="BD93" s="37"/>
-      <c r="BE93" s="37"/>
-      <c r="BF93" s="37"/>
-      <c r="BG93" s="37"/>
-      <c r="BH93" s="37"/>
-      <c r="BI93" s="38"/>
+      <c r="AZ93" s="39"/>
+      <c r="BA93" s="39"/>
+      <c r="BB93" s="39"/>
+      <c r="BC93" s="39"/>
+      <c r="BD93" s="39"/>
+      <c r="BE93" s="39"/>
+      <c r="BF93" s="39"/>
+      <c r="BG93" s="39"/>
+      <c r="BH93" s="39"/>
+      <c r="BI93" s="39"/>
       <c r="CC93" s="36"/>
       <c r="CD93" s="37"/>
       <c r="CE93" s="37"/>
@@ -6742,26 +6740,26 @@
         <v>87</v>
       </c>
       <c r="V94" s="12"/>
-      <c r="AZ94" s="33"/>
-      <c r="BA94" s="34"/>
-      <c r="BB94" s="34"/>
-      <c r="BC94" s="34"/>
-      <c r="BD94" s="34"/>
-      <c r="BE94" s="34"/>
-      <c r="BF94" s="34"/>
-      <c r="BG94" s="34"/>
-      <c r="BH94" s="34"/>
-      <c r="BI94" s="35"/>
-      <c r="CC94" s="33"/>
-      <c r="CD94" s="34"/>
-      <c r="CE94" s="34"/>
-      <c r="CF94" s="34"/>
-      <c r="CG94" s="34"/>
-      <c r="CH94" s="34"/>
-      <c r="CI94" s="34"/>
-      <c r="CJ94" s="34"/>
-      <c r="CK94" s="34"/>
-      <c r="CL94" s="35"/>
+      <c r="AZ94" s="39"/>
+      <c r="BA94" s="39"/>
+      <c r="BB94" s="39"/>
+      <c r="BC94" s="39"/>
+      <c r="BD94" s="39"/>
+      <c r="BE94" s="39"/>
+      <c r="BF94" s="39"/>
+      <c r="BG94" s="39"/>
+      <c r="BH94" s="39"/>
+      <c r="BI94" s="39"/>
+      <c r="CC94" s="27"/>
+      <c r="CD94" s="28"/>
+      <c r="CE94" s="28"/>
+      <c r="CF94" s="28"/>
+      <c r="CG94" s="28"/>
+      <c r="CH94" s="28"/>
+      <c r="CI94" s="28"/>
+      <c r="CJ94" s="28"/>
+      <c r="CK94" s="28"/>
+      <c r="CL94" s="29"/>
       <c r="CM94" s="13"/>
       <c r="CN94" s="2">
         <f t="shared" si="11"/>
@@ -8489,7 +8487,41 @@
       <c r="DH112" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="50">
+    <mergeCell ref="W90:AB91"/>
+    <mergeCell ref="BY31:CK33"/>
+    <mergeCell ref="CC91:CL94"/>
+    <mergeCell ref="CA40:CE41"/>
+    <mergeCell ref="CA43:CE44"/>
+    <mergeCell ref="CA46:CE47"/>
+    <mergeCell ref="CG40:CK41"/>
+    <mergeCell ref="CG43:CK44"/>
+    <mergeCell ref="CG66:CK67"/>
+    <mergeCell ref="CH50:CL51"/>
+    <mergeCell ref="CG54:CK55"/>
+    <mergeCell ref="CG57:CK58"/>
+    <mergeCell ref="CG60:CK61"/>
+    <mergeCell ref="CG63:CK64"/>
+    <mergeCell ref="AP25:BU26"/>
+    <mergeCell ref="AP28:AY29"/>
+    <mergeCell ref="BG46:BP47"/>
+    <mergeCell ref="BG40:BY41"/>
+    <mergeCell ref="BG43:BY44"/>
+    <mergeCell ref="BY22:CB23"/>
+    <mergeCell ref="CJ22:CK23"/>
+    <mergeCell ref="CF22:CG23"/>
+    <mergeCell ref="BY28:CD29"/>
+    <mergeCell ref="CF28:CK29"/>
+    <mergeCell ref="AT36:AV37"/>
+    <mergeCell ref="AP36:AQ37"/>
+    <mergeCell ref="X22:AA23"/>
+    <mergeCell ref="AB22:AL23"/>
+    <mergeCell ref="X25:AA26"/>
+    <mergeCell ref="X28:AA29"/>
+    <mergeCell ref="X31:AA32"/>
+    <mergeCell ref="AB25:AL26"/>
+    <mergeCell ref="AB28:AL29"/>
+    <mergeCell ref="AB31:AL32"/>
     <mergeCell ref="BR18:BV19"/>
     <mergeCell ref="BL18:BQ19"/>
     <mergeCell ref="CA50:CG51"/>
@@ -8506,41 +8538,6 @@
     <mergeCell ref="AV31:BA32"/>
     <mergeCell ref="AH36:AJ37"/>
     <mergeCell ref="AK36:AN37"/>
-    <mergeCell ref="AT36:AV37"/>
-    <mergeCell ref="AP36:AQ37"/>
-    <mergeCell ref="X22:AA23"/>
-    <mergeCell ref="AB22:AL23"/>
-    <mergeCell ref="X25:AA26"/>
-    <mergeCell ref="X28:AA29"/>
-    <mergeCell ref="X31:AA32"/>
-    <mergeCell ref="AB25:AL26"/>
-    <mergeCell ref="AB28:AL29"/>
-    <mergeCell ref="AB31:AL32"/>
-    <mergeCell ref="BY22:CB23"/>
-    <mergeCell ref="CJ22:CK23"/>
-    <mergeCell ref="CF22:CG23"/>
-    <mergeCell ref="BY28:CD29"/>
-    <mergeCell ref="CF28:CK29"/>
-    <mergeCell ref="CG57:CK58"/>
-    <mergeCell ref="CG60:CK61"/>
-    <mergeCell ref="CG63:CK64"/>
-    <mergeCell ref="AP25:BU26"/>
-    <mergeCell ref="AP28:AY29"/>
-    <mergeCell ref="BG46:BP47"/>
-    <mergeCell ref="BG40:BY41"/>
-    <mergeCell ref="BG43:BY44"/>
-    <mergeCell ref="W90:AB91"/>
-    <mergeCell ref="BY31:CK33"/>
-    <mergeCell ref="CC91:CL94"/>
-    <mergeCell ref="AZ91:BI94"/>
-    <mergeCell ref="CA40:CE41"/>
-    <mergeCell ref="CA43:CE44"/>
-    <mergeCell ref="CA46:CE47"/>
-    <mergeCell ref="CG40:CK41"/>
-    <mergeCell ref="CG43:CK44"/>
-    <mergeCell ref="CG66:CK67"/>
-    <mergeCell ref="CH50:CL51"/>
-    <mergeCell ref="CG54:CK55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>